<commit_message>
Getting annual spending for programs
</commit_message>
<xml_diff>
--- a/input_spreadsheets/Master/InputForCode_Master.xlsx
+++ b/input_spreadsheets/Master/InputForCode_Master.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-34840" yWindow="-21140" windowWidth="28460" windowHeight="20120" tabRatio="500" firstSheet="14" activeTab="21" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" tabRatio="500" firstSheet="25" activeTab="27" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Baseline year demographics" sheetId="1" r:id="rId1"/>
@@ -39,9 +39,10 @@
     <sheet name="Program risk areas" sheetId="36" r:id="rId25"/>
     <sheet name="Population risk areas" sheetId="43" r:id="rId26"/>
     <sheet name="Programs annual scale-up" sheetId="51" r:id="rId27"/>
-    <sheet name="Programs cost and coverage" sheetId="20" r:id="rId28"/>
-    <sheet name="Reference programs" sheetId="48" r:id="rId29"/>
-    <sheet name="Programs to include" sheetId="44" r:id="rId30"/>
+    <sheet name="Programs annual spending" sheetId="52" r:id="rId28"/>
+    <sheet name="Programs cost and coverage" sheetId="20" r:id="rId29"/>
+    <sheet name="Reference programs" sheetId="48" r:id="rId30"/>
+    <sheet name="Programs to include" sheetId="44" r:id="rId31"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -2492,7 +2493,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1184" uniqueCount="270">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1292" uniqueCount="273">
   <si>
     <t>year</t>
   </si>
@@ -3302,6 +3303,15 @@
   </si>
   <si>
     <t>Maximum annual scale-up</t>
+  </si>
+  <si>
+    <t>Spending</t>
+  </si>
+  <si>
+    <t>Field</t>
+  </si>
+  <si>
+    <t>Coverage</t>
   </si>
 </sst>
 </file>
@@ -8739,11 +8749,6 @@
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="B36:B38"/>
-    <mergeCell ref="B39:B41"/>
-    <mergeCell ref="B42:B44"/>
-    <mergeCell ref="B45:B47"/>
-    <mergeCell ref="B48:B50"/>
     <mergeCell ref="B25:B27"/>
     <mergeCell ref="B28:B30"/>
     <mergeCell ref="B31:B33"/>
@@ -8754,6 +8759,11 @@
     <mergeCell ref="B14:B16"/>
     <mergeCell ref="B19:B21"/>
     <mergeCell ref="B22:B24"/>
+    <mergeCell ref="B36:B38"/>
+    <mergeCell ref="B39:B41"/>
+    <mergeCell ref="B42:B44"/>
+    <mergeCell ref="B45:B47"/>
+    <mergeCell ref="B48:B50"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -13423,7 +13433,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1500-000000000000}">
   <dimension ref="A1:O53"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="118" workbookViewId="0">
+    <sheetView topLeftCell="A19" zoomScale="85" zoomScaleNormal="118" workbookViewId="0">
       <selection activeCell="O36" sqref="O36"/>
     </sheetView>
   </sheetViews>
@@ -20055,6 +20065,1096 @@
 </file>
 
 <file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD451538-A103-E449-A7A9-980845064FD1}">
+  <dimension ref="A1:Y107"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="56.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:25" x14ac:dyDescent="0.15">
+      <c r="A1" s="9" t="s">
+        <v>203</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>271</v>
+      </c>
+      <c r="C1" s="91">
+        <f>'Baseline year demographics'!$C2+1</f>
+        <v>2017</v>
+      </c>
+      <c r="D1" s="91">
+        <f>C1+1</f>
+        <v>2018</v>
+      </c>
+      <c r="E1" s="91">
+        <f t="shared" ref="E1:P1" si="0">D1+1</f>
+        <v>2019</v>
+      </c>
+      <c r="F1" s="91">
+        <f t="shared" si="0"/>
+        <v>2020</v>
+      </c>
+      <c r="G1" s="91">
+        <f t="shared" si="0"/>
+        <v>2021</v>
+      </c>
+      <c r="H1" s="91">
+        <f t="shared" si="0"/>
+        <v>2022</v>
+      </c>
+      <c r="I1" s="91">
+        <f t="shared" si="0"/>
+        <v>2023</v>
+      </c>
+      <c r="J1" s="91">
+        <f t="shared" si="0"/>
+        <v>2024</v>
+      </c>
+      <c r="K1" s="91">
+        <f t="shared" si="0"/>
+        <v>2025</v>
+      </c>
+      <c r="L1" s="91">
+        <f t="shared" si="0"/>
+        <v>2026</v>
+      </c>
+      <c r="M1" s="91">
+        <f t="shared" si="0"/>
+        <v>2027</v>
+      </c>
+      <c r="N1" s="91">
+        <f t="shared" si="0"/>
+        <v>2028</v>
+      </c>
+      <c r="O1" s="91">
+        <f t="shared" si="0"/>
+        <v>2029</v>
+      </c>
+      <c r="P1" s="91">
+        <f t="shared" si="0"/>
+        <v>2030</v>
+      </c>
+      <c r="Q1" s="91"/>
+      <c r="R1" s="91"/>
+      <c r="S1" s="91"/>
+      <c r="T1" s="91"/>
+      <c r="U1" s="91"/>
+      <c r="V1" s="91"/>
+      <c r="W1" s="91"/>
+      <c r="X1" s="91"/>
+      <c r="Y1" s="91"/>
+    </row>
+    <row r="2" spans="1:25" x14ac:dyDescent="0.15">
+      <c r="A2" t="str">
+        <f>'Programs to include'!A2</f>
+        <v>Balanced energy-protein supplementation</v>
+      </c>
+      <c r="B2" s="122" t="s">
+        <v>270</v>
+      </c>
+      <c r="C2">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:25" x14ac:dyDescent="0.15">
+      <c r="A3" t="str">
+        <f>A2</f>
+        <v>Balanced energy-protein supplementation</v>
+      </c>
+      <c r="B3" s="122" t="s">
+        <v>272</v>
+      </c>
+      <c r="C3">
+        <v>0.1</v>
+      </c>
+      <c r="D3">
+        <v>0.1</v>
+      </c>
+      <c r="E3">
+        <v>0.1</v>
+      </c>
+      <c r="F3">
+        <v>0.1</v>
+      </c>
+      <c r="G3">
+        <v>0.1</v>
+      </c>
+      <c r="H3">
+        <v>0.1</v>
+      </c>
+      <c r="I3">
+        <v>0.1</v>
+      </c>
+      <c r="J3">
+        <v>0.1</v>
+      </c>
+      <c r="K3">
+        <v>0.1</v>
+      </c>
+      <c r="L3">
+        <v>0.1</v>
+      </c>
+      <c r="M3">
+        <v>0.1</v>
+      </c>
+      <c r="N3">
+        <v>0.1</v>
+      </c>
+      <c r="O3">
+        <v>0.1</v>
+      </c>
+      <c r="P3">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:25" x14ac:dyDescent="0.15">
+      <c r="A4" t="str">
+        <f>'Programs to include'!A3</f>
+        <v>Birth age program</v>
+      </c>
+      <c r="B4" s="122" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="5" spans="1:25" x14ac:dyDescent="0.15">
+      <c r="A5" t="str">
+        <f>A4</f>
+        <v>Birth age program</v>
+      </c>
+      <c r="B5" s="122" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="6" spans="1:25" x14ac:dyDescent="0.15">
+      <c r="A6" t="str">
+        <f>'Programs to include'!A4</f>
+        <v>Calcium supplementation</v>
+      </c>
+      <c r="B6" s="122" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="7" spans="1:25" x14ac:dyDescent="0.15">
+      <c r="A7" t="str">
+        <f>A6</f>
+        <v>Calcium supplementation</v>
+      </c>
+      <c r="B7" s="122" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="8" spans="1:25" x14ac:dyDescent="0.15">
+      <c r="A8" t="str">
+        <f>'Programs to include'!A5</f>
+        <v>Cash transfers</v>
+      </c>
+      <c r="B8" s="122" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="9" spans="1:25" x14ac:dyDescent="0.15">
+      <c r="A9" t="str">
+        <f>A8</f>
+        <v>Cash transfers</v>
+      </c>
+      <c r="B9" s="122" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="10" spans="1:25" x14ac:dyDescent="0.15">
+      <c r="A10" t="str">
+        <f>'Programs to include'!A6</f>
+        <v>Family Planning</v>
+      </c>
+      <c r="B10" s="122" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="11" spans="1:25" x14ac:dyDescent="0.15">
+      <c r="A11" t="str">
+        <f>A10</f>
+        <v>Family Planning</v>
+      </c>
+      <c r="B11" s="122" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="12" spans="1:25" x14ac:dyDescent="0.15">
+      <c r="A12" t="str">
+        <f>'Programs to include'!A7</f>
+        <v>IFA fortification of maize</v>
+      </c>
+      <c r="B12" s="122" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="13" spans="1:25" x14ac:dyDescent="0.15">
+      <c r="A13" t="str">
+        <f>A12</f>
+        <v>IFA fortification of maize</v>
+      </c>
+      <c r="B13" s="122" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="14" spans="1:25" x14ac:dyDescent="0.15">
+      <c r="A14" t="str">
+        <f>'Programs to include'!A8</f>
+        <v>IFA fortification of rice</v>
+      </c>
+      <c r="B14" s="122" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="15" spans="1:25" x14ac:dyDescent="0.15">
+      <c r="A15" t="str">
+        <f>A14</f>
+        <v>IFA fortification of rice</v>
+      </c>
+      <c r="B15" s="122" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="16" spans="1:25" x14ac:dyDescent="0.15">
+      <c r="A16" t="str">
+        <f>'Programs to include'!A9</f>
+        <v>IFA fortification of wheat flour</v>
+      </c>
+      <c r="B16" s="122" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A17" t="str">
+        <f>A16</f>
+        <v>IFA fortification of wheat flour</v>
+      </c>
+      <c r="B17" s="122" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A18" t="str">
+        <f>'Programs to include'!A10</f>
+        <v>IFAS not poor: community</v>
+      </c>
+      <c r="B18" s="122" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A19" t="str">
+        <f>A18</f>
+        <v>IFAS not poor: community</v>
+      </c>
+      <c r="B19" s="122" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A20" t="str">
+        <f>'Programs to include'!A11</f>
+        <v>IFAS not poor: community (malaria area)</v>
+      </c>
+      <c r="B20" s="122" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A21" t="str">
+        <f>A20</f>
+        <v>IFAS not poor: community (malaria area)</v>
+      </c>
+      <c r="B21" s="122" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A22" t="str">
+        <f>'Programs to include'!A12</f>
+        <v>IFAS not poor: hospital</v>
+      </c>
+      <c r="B22" s="122" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A23" t="str">
+        <f>A22</f>
+        <v>IFAS not poor: hospital</v>
+      </c>
+      <c r="B23" s="122" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A24" t="str">
+        <f>'Programs to include'!A13</f>
+        <v>IFAS not poor: hospital (malaria area)</v>
+      </c>
+      <c r="B24" s="122" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A25" t="str">
+        <f>A24</f>
+        <v>IFAS not poor: hospital (malaria area)</v>
+      </c>
+      <c r="B25" s="122" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A26" t="str">
+        <f>'Programs to include'!A14</f>
+        <v>IFAS not poor: retailer</v>
+      </c>
+      <c r="B26" s="122" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A27" t="str">
+        <f>A26</f>
+        <v>IFAS not poor: retailer</v>
+      </c>
+      <c r="B27" s="122" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A28" t="str">
+        <f>'Programs to include'!A15</f>
+        <v>IFAS not poor: retailer (malaria area)</v>
+      </c>
+      <c r="B28" s="122" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A29" t="str">
+        <f>A28</f>
+        <v>IFAS not poor: retailer (malaria area)</v>
+      </c>
+      <c r="B29" s="122" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A30" t="str">
+        <f>'Programs to include'!A16</f>
+        <v>IFAS not poor: school</v>
+      </c>
+      <c r="B30" s="122" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A31" t="str">
+        <f>A30</f>
+        <v>IFAS not poor: school</v>
+      </c>
+      <c r="B31" s="122" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A32" t="str">
+        <f>'Programs to include'!A17</f>
+        <v>IFAS not poor: school (malaria area)</v>
+      </c>
+      <c r="B32" s="122" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A33" t="str">
+        <f>A32</f>
+        <v>IFAS not poor: school (malaria area)</v>
+      </c>
+      <c r="B33" s="122" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A34" t="str">
+        <f>'Programs to include'!A18</f>
+        <v>IFAS poor: community</v>
+      </c>
+      <c r="B34" s="122" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A35" t="str">
+        <f>A34</f>
+        <v>IFAS poor: community</v>
+      </c>
+      <c r="B35" s="122" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A36" t="str">
+        <f>'Programs to include'!A19</f>
+        <v>IFAS poor: community (malaria area)</v>
+      </c>
+      <c r="B36" s="122" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A37" t="str">
+        <f>A36</f>
+        <v>IFAS poor: community (malaria area)</v>
+      </c>
+      <c r="B37" s="122" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A38" t="str">
+        <f>'Programs to include'!A20</f>
+        <v>IFAS poor: hospital</v>
+      </c>
+      <c r="B38" s="122" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A39" t="str">
+        <f>A38</f>
+        <v>IFAS poor: hospital</v>
+      </c>
+      <c r="B39" s="122" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A40" t="str">
+        <f>'Programs to include'!A21</f>
+        <v>IFAS poor: hospital (malaria area)</v>
+      </c>
+      <c r="B40" s="122" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A41" t="str">
+        <f>A40</f>
+        <v>IFAS poor: hospital (malaria area)</v>
+      </c>
+      <c r="B41" s="122" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A42" t="str">
+        <f>'Programs to include'!A22</f>
+        <v>IFAS poor: school</v>
+      </c>
+      <c r="B42" s="122" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A43" t="str">
+        <f>A42</f>
+        <v>IFAS poor: school</v>
+      </c>
+      <c r="B43" s="122" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A44" t="str">
+        <f>'Programs to include'!A23</f>
+        <v>IFAS poor: school (malaria area)</v>
+      </c>
+      <c r="B44" s="122" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A45" t="str">
+        <f>A44</f>
+        <v>IFAS poor: school (malaria area)</v>
+      </c>
+      <c r="B45" s="122" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A46" t="str">
+        <f>'Programs to include'!A24</f>
+        <v>IPTp</v>
+      </c>
+      <c r="B46" s="122" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A47" t="str">
+        <f>A46</f>
+        <v>IPTp</v>
+      </c>
+      <c r="B47" s="122" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A48" t="str">
+        <f>'Programs to include'!A25</f>
+        <v>Iron and folic acid supplementation for pregnant women</v>
+      </c>
+      <c r="B48" s="122" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A49" t="str">
+        <f>A48</f>
+        <v>Iron and folic acid supplementation for pregnant women</v>
+      </c>
+      <c r="B49" s="122" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A50" t="str">
+        <f>'Programs to include'!A26</f>
+        <v>Iron and folic acid supplementation for pregnant women (malaria area)</v>
+      </c>
+      <c r="B50" s="122" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A51" t="str">
+        <f>A50</f>
+        <v>Iron and folic acid supplementation for pregnant women (malaria area)</v>
+      </c>
+      <c r="B51" s="122" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A52" t="str">
+        <f>'Programs to include'!A27</f>
+        <v>Iron and iodine fortification of salt</v>
+      </c>
+      <c r="B52" s="122" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A53" t="str">
+        <f>A52</f>
+        <v>Iron and iodine fortification of salt</v>
+      </c>
+      <c r="B53" s="122" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A54" t="str">
+        <f>'Programs to include'!A28</f>
+        <v>Iron fortification of maize</v>
+      </c>
+      <c r="B54" s="122" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A55" t="str">
+        <f>A54</f>
+        <v>Iron fortification of maize</v>
+      </c>
+      <c r="B55" s="122" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A56" t="str">
+        <f>'Programs to include'!A29</f>
+        <v>Iron fortification of rice</v>
+      </c>
+      <c r="B56" s="122" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A57" t="str">
+        <f>A56</f>
+        <v>Iron fortification of rice</v>
+      </c>
+      <c r="B57" s="122" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A58" t="str">
+        <f>'Programs to include'!A30</f>
+        <v>Iron fortification of wheat flour</v>
+      </c>
+      <c r="B58" s="122" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A59" t="str">
+        <f>A58</f>
+        <v>Iron fortification of wheat flour</v>
+      </c>
+      <c r="B59" s="122" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A60" t="str">
+        <f>'Programs to include'!A31</f>
+        <v>Long-lasting insecticide-treated bednets</v>
+      </c>
+      <c r="B60" s="122" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A61" t="str">
+        <f>A60</f>
+        <v>Long-lasting insecticide-treated bednets</v>
+      </c>
+      <c r="B61" s="122" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A62" t="str">
+        <f>'Programs to include'!A32</f>
+        <v>Mg for eclampsia</v>
+      </c>
+      <c r="B62" s="122" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A63" t="str">
+        <f>A62</f>
+        <v>Mg for eclampsia</v>
+      </c>
+      <c r="B63" s="122" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A64" t="str">
+        <f>'Programs to include'!A33</f>
+        <v>Mg for pre-eclampsia</v>
+      </c>
+      <c r="B64" s="122" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A65" t="str">
+        <f>A64</f>
+        <v>Mg for pre-eclampsia</v>
+      </c>
+      <c r="B65" s="122" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A66" t="str">
+        <f>'Programs to include'!A34</f>
+        <v>Multiple micronutrient supplementation</v>
+      </c>
+      <c r="B66" s="122" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A67" t="str">
+        <f>A66</f>
+        <v>Multiple micronutrient supplementation</v>
+      </c>
+      <c r="B67" s="122" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A68" t="str">
+        <f>'Programs to include'!A35</f>
+        <v>Multiple micronutrient supplementation (malaria area)</v>
+      </c>
+      <c r="B68" s="122" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A69" t="str">
+        <f>A68</f>
+        <v>Multiple micronutrient supplementation (malaria area)</v>
+      </c>
+      <c r="B69" s="122" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A70" t="str">
+        <f>'Programs to include'!A36</f>
+        <v>Oral rehydration salts</v>
+      </c>
+      <c r="B70" s="122" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A71" t="str">
+        <f>A70</f>
+        <v>Oral rehydration salts</v>
+      </c>
+      <c r="B71" s="122" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A72" t="str">
+        <f>'Programs to include'!A37</f>
+        <v>Public provision of complementary foods</v>
+      </c>
+      <c r="B72" s="122" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A73" t="str">
+        <f>A72</f>
+        <v>Public provision of complementary foods</v>
+      </c>
+      <c r="B73" s="122" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A74" t="str">
+        <f>'Programs to include'!A38</f>
+        <v>Public provision of complementary foods with iron</v>
+      </c>
+      <c r="B74" s="122" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A75" t="str">
+        <f>A74</f>
+        <v>Public provision of complementary foods with iron</v>
+      </c>
+      <c r="B75" s="122" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A76" t="str">
+        <f>'Programs to include'!A39</f>
+        <v>Public provision of complementary foods with iron (malaria area)</v>
+      </c>
+      <c r="B76" s="122" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A77" t="str">
+        <f>A76</f>
+        <v>Public provision of complementary foods with iron (malaria area)</v>
+      </c>
+      <c r="B77" s="122" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A78" t="str">
+        <f>'Programs to include'!A40</f>
+        <v>Sprinkles</v>
+      </c>
+      <c r="B78" s="122" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A79" t="str">
+        <f>A78</f>
+        <v>Sprinkles</v>
+      </c>
+      <c r="B79" s="122" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A80" t="str">
+        <f>'Programs to include'!A41</f>
+        <v>Sprinkles (malaria area)</v>
+      </c>
+      <c r="B80" s="122" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A81" t="str">
+        <f>A80</f>
+        <v>Sprinkles (malaria area)</v>
+      </c>
+      <c r="B81" s="122" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A82" t="str">
+        <f>'Programs to include'!A42</f>
+        <v>Treatment of MAM</v>
+      </c>
+      <c r="B82" s="122" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A83" t="str">
+        <f>A82</f>
+        <v>Treatment of MAM</v>
+      </c>
+      <c r="B83" s="122" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A84" t="str">
+        <f>'Programs to include'!A43</f>
+        <v>Treatment of SAM</v>
+      </c>
+      <c r="B84" s="122" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A85" t="str">
+        <f>A84</f>
+        <v>Treatment of SAM</v>
+      </c>
+      <c r="B85" s="122" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A86" t="str">
+        <f>'Programs to include'!A44</f>
+        <v>Vitamin A supplementation</v>
+      </c>
+      <c r="B86" s="122" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A87" t="str">
+        <f>A86</f>
+        <v>Vitamin A supplementation</v>
+      </c>
+      <c r="B87" s="122" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A88" t="str">
+        <f>'Programs to include'!A45</f>
+        <v>WASH: Handwashing</v>
+      </c>
+      <c r="B88" s="122" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A89" t="str">
+        <f>A88</f>
+        <v>WASH: Handwashing</v>
+      </c>
+      <c r="B89" s="122" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A90" t="str">
+        <f>'Programs to include'!A46</f>
+        <v>WASH: Hygenic disposal</v>
+      </c>
+      <c r="B90" s="122" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A91" t="str">
+        <f>A90</f>
+        <v>WASH: Hygenic disposal</v>
+      </c>
+      <c r="B91" s="122" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A92" t="str">
+        <f>'Programs to include'!A47</f>
+        <v>WASH: Improved sanitation</v>
+      </c>
+      <c r="B92" s="122" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A93" t="str">
+        <f>A92</f>
+        <v>WASH: Improved sanitation</v>
+      </c>
+      <c r="B93" s="122" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A94" t="str">
+        <f>'Programs to include'!A48</f>
+        <v>WASH: Improved water source</v>
+      </c>
+      <c r="B94" s="122" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A95" t="str">
+        <f>A94</f>
+        <v>WASH: Improved water source</v>
+      </c>
+      <c r="B95" s="122" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A96" t="str">
+        <f>'Programs to include'!A49</f>
+        <v>WASH: Piped water</v>
+      </c>
+      <c r="B96" s="122" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A97" t="str">
+        <f>A96</f>
+        <v>WASH: Piped water</v>
+      </c>
+      <c r="B97" s="122" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A98" t="str">
+        <f>'Programs to include'!A50</f>
+        <v>Zinc for treatment + ORS</v>
+      </c>
+      <c r="B98" s="122" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A99" t="str">
+        <f>A98</f>
+        <v>Zinc for treatment + ORS</v>
+      </c>
+      <c r="B99" s="122" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A100" t="str">
+        <f>'Programs to include'!A51</f>
+        <v>Zinc supplementation</v>
+      </c>
+      <c r="B100" s="122" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A101" t="str">
+        <f>A100</f>
+        <v>Zinc supplementation</v>
+      </c>
+      <c r="B101" s="122" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A102" t="str">
+        <f>'Programs to include'!A52</f>
+        <v>IYCF 1</v>
+      </c>
+      <c r="B102" s="122" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A103" t="str">
+        <f>A102</f>
+        <v>IYCF 1</v>
+      </c>
+      <c r="B103" s="122" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A104" t="str">
+        <f>'Programs to include'!A53</f>
+        <v>IYCF 2</v>
+      </c>
+      <c r="B104" s="122" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A105" t="str">
+        <f>A104</f>
+        <v>IYCF 2</v>
+      </c>
+      <c r="B105" s="122" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A106" t="str">
+        <f>'Programs to include'!A54</f>
+        <v>IYCF 3</v>
+      </c>
+      <c r="B106" s="122" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A107" t="str">
+        <f>A106</f>
+        <v>IYCF 3</v>
+      </c>
+      <c r="B107" s="122" t="s">
+        <v>272</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1A00-000000000000}">
   <dimension ref="A1:E54"/>
   <sheetViews>
@@ -20906,71 +22006,6 @@
   </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4FD8166B-8704-DF4E-9AA8-4565893AE0CB}">
-  <dimension ref="A1:B9"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
-  <cols>
-    <col min="1" max="1" width="28.6640625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A1" s="9" t="s">
-        <v>203</v>
-      </c>
-      <c r="B1" s="9"/>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A2" s="122" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A3" s="122" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A4" s="4" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A5" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A6" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A7" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A8" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A9" t="s">
-        <v>257</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -21896,6 +22931,71 @@
 </file>
 
 <file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4FD8166B-8704-DF4E-9AA8-4565893AE0CB}">
+  <dimension ref="A1:B9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="28.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A1" s="9" t="s">
+        <v>203</v>
+      </c>
+      <c r="B1" s="9"/>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A2" s="122" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A3" s="122" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A4" s="4" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A5" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A6" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A7" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A8" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A9" t="s">
+        <v>257</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1B00-000000000000}">
   <sheetPr>
     <tabColor theme="9" tint="-0.249977111117893"/>

</xml_diff>

<commit_message>
Functions to read and interpolate annual coverage for programs
</commit_message>
<xml_diff>
--- a/input_spreadsheets/Master/InputForCode_Master.xlsx
+++ b/input_spreadsheets/Master/InputForCode_Master.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" tabRatio="500" firstSheet="25" activeTab="27" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" tabRatio="500" firstSheet="25" activeTab="28" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Baseline year demographics" sheetId="1" r:id="rId1"/>
@@ -20068,8 +20068,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD451538-A103-E449-A7A9-980845064FD1}">
   <dimension ref="A1:Y107"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="C87" sqref="C87:L87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -20158,8 +20158,11 @@
       <c r="B2" s="122" t="s">
         <v>270</v>
       </c>
-      <c r="C2">
-        <v>100000</v>
+      <c r="E2">
+        <v>10000</v>
+      </c>
+      <c r="G2">
+        <v>300000</v>
       </c>
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.15">
@@ -20170,18 +20173,12 @@
       <c r="B3" s="122" t="s">
         <v>272</v>
       </c>
-      <c r="C3">
-        <v>0.1</v>
-      </c>
       <c r="D3">
         <v>0.1</v>
       </c>
       <c r="E3">
         <v>0.1</v>
       </c>
-      <c r="F3">
-        <v>0.1</v>
-      </c>
       <c r="G3">
         <v>0.1</v>
       </c>
@@ -20198,19 +20195,7 @@
         <v>0.1</v>
       </c>
       <c r="L3">
-        <v>0.1</v>
-      </c>
-      <c r="M3">
-        <v>0.1</v>
-      </c>
-      <c r="N3">
-        <v>0.1</v>
-      </c>
-      <c r="O3">
-        <v>0.1</v>
-      </c>
-      <c r="P3">
-        <v>0.1</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.15">
@@ -20906,7 +20891,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="81" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A81" t="str">
         <f>A80</f>
         <v>Sprinkles (malaria area)</v>
@@ -20915,7 +20900,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="82" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A82" t="str">
         <f>'Programs to include'!A42</f>
         <v>Treatment of MAM</v>
@@ -20924,7 +20909,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="83" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A83" t="str">
         <f>A82</f>
         <v>Treatment of MAM</v>
@@ -20933,7 +20918,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="84" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A84" t="str">
         <f>'Programs to include'!A43</f>
         <v>Treatment of SAM</v>
@@ -20942,7 +20927,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="85" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A85" t="str">
         <f>A84</f>
         <v>Treatment of SAM</v>
@@ -20951,7 +20936,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="86" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A86" t="str">
         <f>'Programs to include'!A44</f>
         <v>Vitamin A supplementation</v>
@@ -20960,7 +20945,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="87" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A87" t="str">
         <f>A86</f>
         <v>Vitamin A supplementation</v>
@@ -20968,8 +20953,32 @@
       <c r="B87" s="122" t="s">
         <v>272</v>
       </c>
-    </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="D87">
+        <v>0.1</v>
+      </c>
+      <c r="E87">
+        <v>0.1</v>
+      </c>
+      <c r="G87">
+        <v>0.1</v>
+      </c>
+      <c r="H87">
+        <v>0.1</v>
+      </c>
+      <c r="I87">
+        <v>0.1</v>
+      </c>
+      <c r="J87">
+        <v>0.1</v>
+      </c>
+      <c r="K87">
+        <v>0.1</v>
+      </c>
+      <c r="L87">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="88" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A88" t="str">
         <f>'Programs to include'!A45</f>
         <v>WASH: Handwashing</v>
@@ -20978,7 +20987,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="89" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A89" t="str">
         <f>A88</f>
         <v>WASH: Handwashing</v>
@@ -20987,7 +20996,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="90" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A90" t="str">
         <f>'Programs to include'!A46</f>
         <v>WASH: Hygenic disposal</v>
@@ -20996,7 +21005,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="91" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A91" t="str">
         <f>A90</f>
         <v>WASH: Hygenic disposal</v>
@@ -21005,7 +21014,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="92" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A92" t="str">
         <f>'Programs to include'!A47</f>
         <v>WASH: Improved sanitation</v>
@@ -21014,7 +21023,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="93" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A93" t="str">
         <f>A92</f>
         <v>WASH: Improved sanitation</v>
@@ -21023,7 +21032,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="94" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A94" t="str">
         <f>'Programs to include'!A48</f>
         <v>WASH: Improved water source</v>
@@ -21032,7 +21041,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="95" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A95" t="str">
         <f>A94</f>
         <v>WASH: Improved water source</v>
@@ -21041,7 +21050,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="96" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A96" t="str">
         <f>'Programs to include'!A49</f>
         <v>WASH: Piped water</v>
@@ -21158,8 +21167,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1A00-000000000000}">
   <dimension ref="A1:E54"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="B44" sqref="B44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>

</xml_diff>

<commit_message>
Script to run the master workbook
</commit_message>
<xml_diff>
--- a/input_spreadsheets/Master/InputForCode_Master.xlsx
+++ b/input_spreadsheets/Master/InputForCode_Master.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" tabRatio="500" firstSheet="23" activeTab="28" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-20" yWindow="460" windowWidth="25600" windowHeight="15540" tabRatio="500" firstSheet="25" activeTab="30" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Baseline year demographics" sheetId="1" r:id="rId1"/>
@@ -1794,6 +1794,49 @@
 </comments>
 </file>
 
+<file path=xl/comments21.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Sam</author>
+  </authors>
+  <commentList>
+    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{23C0022E-2DA6-F34A-B642-FED244052CCA}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Sam:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>This is the calibration year and uses baseline coverage.</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
@@ -2493,7 +2536,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1292" uniqueCount="273">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1245" uniqueCount="273">
   <si>
     <t>year</t>
   </si>
@@ -6777,7 +6820,7 @@
   <dimension ref="A1:E57"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -7219,7 +7262,7 @@
   <dimension ref="A1:G22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -9571,7 +9614,7 @@
   <dimension ref="A1:O43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -11121,7 +11164,7 @@
   <dimension ref="A1:I52"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A51" sqref="A51"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -13433,8 +13476,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1500-000000000000}">
   <dimension ref="A1:O53"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" zoomScale="85" zoomScaleNormal="118" workbookViewId="0">
-      <selection activeCell="O36" sqref="O36"/>
+    <sheetView zoomScale="85" zoomScaleNormal="118" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -18666,8 +18709,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1800-000000000000}">
   <dimension ref="A1:K54"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A54"/>
+    <sheetView topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="E46" sqref="E46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -19563,8 +19606,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DBC6050C-0865-7046-B5F3-F185B3ED8E81}">
   <dimension ref="A1:B54"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="A44" sqref="A44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -20065,16 +20108,17 @@
 </file>
 
 <file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD451538-A103-E449-A7A9-980845064FD1}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD451538-A103-E449-A7A9-980845064FD1}">
   <dimension ref="A1:Y107"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F92" sqref="F92"/>
+    <sheetView topLeftCell="A63" workbookViewId="0">
+      <selection activeCell="D73" sqref="D73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="56.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:25" x14ac:dyDescent="0.15">
@@ -20158,6 +20202,7 @@
       <c r="B2" s="122" t="s">
         <v>270</v>
       </c>
+      <c r="C2" s="34"/>
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A3" t="str">
@@ -20167,6 +20212,7 @@
       <c r="B3" s="122" t="s">
         <v>272</v>
       </c>
+      <c r="C3" s="34"/>
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A4" t="str">
@@ -20176,6 +20222,7 @@
       <c r="B4" s="122" t="s">
         <v>270</v>
       </c>
+      <c r="C4" s="34"/>
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A5" t="str">
@@ -20185,6 +20232,7 @@
       <c r="B5" s="122" t="s">
         <v>272</v>
       </c>
+      <c r="C5" s="34"/>
     </row>
     <row r="6" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A6" t="str">
@@ -20194,6 +20242,7 @@
       <c r="B6" s="122" t="s">
         <v>270</v>
       </c>
+      <c r="C6" s="34"/>
     </row>
     <row r="7" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A7" t="str">
@@ -20203,6 +20252,7 @@
       <c r="B7" s="122" t="s">
         <v>272</v>
       </c>
+      <c r="C7" s="34"/>
     </row>
     <row r="8" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A8" t="str">
@@ -20212,6 +20262,7 @@
       <c r="B8" s="122" t="s">
         <v>270</v>
       </c>
+      <c r="C8" s="34"/>
     </row>
     <row r="9" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A9" t="str">
@@ -20221,6 +20272,7 @@
       <c r="B9" s="122" t="s">
         <v>272</v>
       </c>
+      <c r="C9" s="34"/>
     </row>
     <row r="10" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A10" t="str">
@@ -20230,6 +20282,7 @@
       <c r="B10" s="122" t="s">
         <v>270</v>
       </c>
+      <c r="C10" s="34"/>
     </row>
     <row r="11" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A11" t="str">
@@ -20239,6 +20292,7 @@
       <c r="B11" s="122" t="s">
         <v>272</v>
       </c>
+      <c r="C11" s="34"/>
     </row>
     <row r="12" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A12" t="str">
@@ -20248,6 +20302,7 @@
       <c r="B12" s="122" t="s">
         <v>270</v>
       </c>
+      <c r="C12" s="34"/>
     </row>
     <row r="13" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A13" t="str">
@@ -20257,6 +20312,7 @@
       <c r="B13" s="122" t="s">
         <v>272</v>
       </c>
+      <c r="C13" s="34"/>
     </row>
     <row r="14" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A14" t="str">
@@ -20266,6 +20322,7 @@
       <c r="B14" s="122" t="s">
         <v>270</v>
       </c>
+      <c r="C14" s="34"/>
     </row>
     <row r="15" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A15" t="str">
@@ -20275,6 +20332,7 @@
       <c r="B15" s="122" t="s">
         <v>272</v>
       </c>
+      <c r="C15" s="34"/>
     </row>
     <row r="16" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A16" t="str">
@@ -20284,8 +20342,9 @@
       <c r="B16" s="122" t="s">
         <v>270</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="C16" s="34"/>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A17" t="str">
         <f>A16</f>
         <v>IFA fortification of wheat flour</v>
@@ -20293,8 +20352,9 @@
       <c r="B17" s="122" t="s">
         <v>272</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="C17" s="34"/>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A18" t="str">
         <f>'Programs to include'!A10</f>
         <v>IFAS not poor: community</v>
@@ -20302,8 +20362,9 @@
       <c r="B18" s="122" t="s">
         <v>270</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="C18" s="34"/>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A19" t="str">
         <f>A18</f>
         <v>IFAS not poor: community</v>
@@ -20311,8 +20372,9 @@
       <c r="B19" s="122" t="s">
         <v>272</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="C19" s="34"/>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A20" t="str">
         <f>'Programs to include'!A11</f>
         <v>IFAS not poor: community (malaria area)</v>
@@ -20320,8 +20382,9 @@
       <c r="B20" s="122" t="s">
         <v>270</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="C20" s="34"/>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A21" t="str">
         <f>A20</f>
         <v>IFAS not poor: community (malaria area)</v>
@@ -20329,8 +20392,9 @@
       <c r="B21" s="122" t="s">
         <v>272</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="C21" s="34"/>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A22" t="str">
         <f>'Programs to include'!A12</f>
         <v>IFAS not poor: hospital</v>
@@ -20338,8 +20402,9 @@
       <c r="B22" s="122" t="s">
         <v>270</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="C22" s="34"/>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A23" t="str">
         <f>A22</f>
         <v>IFAS not poor: hospital</v>
@@ -20347,8 +20412,9 @@
       <c r="B23" s="122" t="s">
         <v>272</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="C23" s="34"/>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A24" t="str">
         <f>'Programs to include'!A13</f>
         <v>IFAS not poor: hospital (malaria area)</v>
@@ -20356,8 +20422,9 @@
       <c r="B24" s="122" t="s">
         <v>270</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="C24" s="34"/>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A25" t="str">
         <f>A24</f>
         <v>IFAS not poor: hospital (malaria area)</v>
@@ -20365,8 +20432,9 @@
       <c r="B25" s="122" t="s">
         <v>272</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="C25" s="34"/>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A26" t="str">
         <f>'Programs to include'!A14</f>
         <v>IFAS not poor: retailer</v>
@@ -20374,8 +20442,9 @@
       <c r="B26" s="122" t="s">
         <v>270</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="C26" s="34"/>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A27" t="str">
         <f>A26</f>
         <v>IFAS not poor: retailer</v>
@@ -20383,8 +20452,9 @@
       <c r="B27" s="122" t="s">
         <v>272</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="C27" s="34"/>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A28" t="str">
         <f>'Programs to include'!A15</f>
         <v>IFAS not poor: retailer (malaria area)</v>
@@ -20392,8 +20462,9 @@
       <c r="B28" s="122" t="s">
         <v>270</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="C28" s="34"/>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A29" t="str">
         <f>A28</f>
         <v>IFAS not poor: retailer (malaria area)</v>
@@ -20401,8 +20472,9 @@
       <c r="B29" s="122" t="s">
         <v>272</v>
       </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="C29" s="34"/>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A30" t="str">
         <f>'Programs to include'!A16</f>
         <v>IFAS not poor: school</v>
@@ -20410,8 +20482,9 @@
       <c r="B30" s="122" t="s">
         <v>270</v>
       </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="C30" s="34"/>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A31" t="str">
         <f>A30</f>
         <v>IFAS not poor: school</v>
@@ -20419,8 +20492,9 @@
       <c r="B31" s="122" t="s">
         <v>272</v>
       </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="C31" s="34"/>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A32" t="str">
         <f>'Programs to include'!A17</f>
         <v>IFAS not poor: school (malaria area)</v>
@@ -20428,8 +20502,9 @@
       <c r="B32" s="122" t="s">
         <v>270</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="C32" s="34"/>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A33" t="str">
         <f>A32</f>
         <v>IFAS not poor: school (malaria area)</v>
@@ -20437,8 +20512,9 @@
       <c r="B33" s="122" t="s">
         <v>272</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="C33" s="34"/>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A34" t="str">
         <f>'Programs to include'!A18</f>
         <v>IFAS poor: community</v>
@@ -20446,8 +20522,9 @@
       <c r="B34" s="122" t="s">
         <v>270</v>
       </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="C34" s="34"/>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A35" t="str">
         <f>A34</f>
         <v>IFAS poor: community</v>
@@ -20455,8 +20532,9 @@
       <c r="B35" s="122" t="s">
         <v>272</v>
       </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="C35" s="34"/>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A36" t="str">
         <f>'Programs to include'!A19</f>
         <v>IFAS poor: community (malaria area)</v>
@@ -20464,8 +20542,9 @@
       <c r="B36" s="122" t="s">
         <v>270</v>
       </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="C36" s="34"/>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A37" t="str">
         <f>A36</f>
         <v>IFAS poor: community (malaria area)</v>
@@ -20473,8 +20552,9 @@
       <c r="B37" s="122" t="s">
         <v>272</v>
       </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="C37" s="34"/>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A38" t="str">
         <f>'Programs to include'!A20</f>
         <v>IFAS poor: hospital</v>
@@ -20482,8 +20562,9 @@
       <c r="B38" s="122" t="s">
         <v>270</v>
       </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="C38" s="34"/>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A39" t="str">
         <f>A38</f>
         <v>IFAS poor: hospital</v>
@@ -20491,8 +20572,9 @@
       <c r="B39" s="122" t="s">
         <v>272</v>
       </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="C39" s="34"/>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A40" t="str">
         <f>'Programs to include'!A21</f>
         <v>IFAS poor: hospital (malaria area)</v>
@@ -20500,8 +20582,9 @@
       <c r="B40" s="122" t="s">
         <v>270</v>
       </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="C40" s="34"/>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A41" t="str">
         <f>A40</f>
         <v>IFAS poor: hospital (malaria area)</v>
@@ -20509,8 +20592,9 @@
       <c r="B41" s="122" t="s">
         <v>272</v>
       </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="C41" s="34"/>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A42" t="str">
         <f>'Programs to include'!A22</f>
         <v>IFAS poor: school</v>
@@ -20518,8 +20602,9 @@
       <c r="B42" s="122" t="s">
         <v>270</v>
       </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="C42" s="34"/>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A43" t="str">
         <f>A42</f>
         <v>IFAS poor: school</v>
@@ -20527,8 +20612,9 @@
       <c r="B43" s="122" t="s">
         <v>272</v>
       </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="C43" s="34"/>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A44" t="str">
         <f>'Programs to include'!A23</f>
         <v>IFAS poor: school (malaria area)</v>
@@ -20536,8 +20622,9 @@
       <c r="B44" s="122" t="s">
         <v>270</v>
       </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="C44" s="34"/>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A45" t="str">
         <f>A44</f>
         <v>IFAS poor: school (malaria area)</v>
@@ -20545,8 +20632,9 @@
       <c r="B45" s="122" t="s">
         <v>272</v>
       </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="C45" s="34"/>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A46" t="str">
         <f>'Programs to include'!A24</f>
         <v>IPTp</v>
@@ -20554,8 +20642,9 @@
       <c r="B46" s="122" t="s">
         <v>270</v>
       </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="C46" s="34"/>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A47" t="str">
         <f>A46</f>
         <v>IPTp</v>
@@ -20563,8 +20652,9 @@
       <c r="B47" s="122" t="s">
         <v>272</v>
       </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="C47" s="34"/>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A48" t="str">
         <f>'Programs to include'!A25</f>
         <v>Iron and folic acid supplementation for pregnant women</v>
@@ -20572,8 +20662,9 @@
       <c r="B48" s="122" t="s">
         <v>270</v>
       </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="C48" s="34"/>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A49" t="str">
         <f>A48</f>
         <v>Iron and folic acid supplementation for pregnant women</v>
@@ -20581,8 +20672,9 @@
       <c r="B49" s="122" t="s">
         <v>272</v>
       </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="C49" s="34"/>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A50" t="str">
         <f>'Programs to include'!A26</f>
         <v>Iron and folic acid supplementation for pregnant women (malaria area)</v>
@@ -20590,8 +20682,9 @@
       <c r="B50" s="122" t="s">
         <v>270</v>
       </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="C50" s="34"/>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A51" t="str">
         <f>A50</f>
         <v>Iron and folic acid supplementation for pregnant women (malaria area)</v>
@@ -20599,8 +20692,9 @@
       <c r="B51" s="122" t="s">
         <v>272</v>
       </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="C51" s="34"/>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A52" t="str">
         <f>'Programs to include'!A27</f>
         <v>Iron and iodine fortification of salt</v>
@@ -20608,8 +20702,9 @@
       <c r="B52" s="122" t="s">
         <v>270</v>
       </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="C52" s="34"/>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A53" t="str">
         <f>A52</f>
         <v>Iron and iodine fortification of salt</v>
@@ -20617,8 +20712,9 @@
       <c r="B53" s="122" t="s">
         <v>272</v>
       </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="C53" s="34"/>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A54" t="str">
         <f>'Programs to include'!A28</f>
         <v>Iron fortification of maize</v>
@@ -20626,8 +20722,9 @@
       <c r="B54" s="122" t="s">
         <v>270</v>
       </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="C54" s="34"/>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A55" t="str">
         <f>A54</f>
         <v>Iron fortification of maize</v>
@@ -20635,8 +20732,9 @@
       <c r="B55" s="122" t="s">
         <v>272</v>
       </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="C55" s="34"/>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A56" t="str">
         <f>'Programs to include'!A29</f>
         <v>Iron fortification of rice</v>
@@ -20644,8 +20742,9 @@
       <c r="B56" s="122" t="s">
         <v>270</v>
       </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="C56" s="34"/>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A57" t="str">
         <f>A56</f>
         <v>Iron fortification of rice</v>
@@ -20653,8 +20752,9 @@
       <c r="B57" s="122" t="s">
         <v>272</v>
       </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="C57" s="34"/>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A58" t="str">
         <f>'Programs to include'!A30</f>
         <v>Iron fortification of wheat flour</v>
@@ -20662,8 +20762,9 @@
       <c r="B58" s="122" t="s">
         <v>270</v>
       </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="C58" s="34"/>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A59" t="str">
         <f>A58</f>
         <v>Iron fortification of wheat flour</v>
@@ -20671,8 +20772,9 @@
       <c r="B59" s="122" t="s">
         <v>272</v>
       </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="C59" s="34"/>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A60" t="str">
         <f>'Programs to include'!A31</f>
         <v>Long-lasting insecticide-treated bednets</v>
@@ -20680,8 +20782,9 @@
       <c r="B60" s="122" t="s">
         <v>270</v>
       </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="C60" s="34"/>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A61" t="str">
         <f>A60</f>
         <v>Long-lasting insecticide-treated bednets</v>
@@ -20689,8 +20792,9 @@
       <c r="B61" s="122" t="s">
         <v>272</v>
       </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="C61" s="34"/>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A62" t="str">
         <f>'Programs to include'!A32</f>
         <v>Mg for eclampsia</v>
@@ -20698,8 +20802,9 @@
       <c r="B62" s="122" t="s">
         <v>270</v>
       </c>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="C62" s="34"/>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A63" t="str">
         <f>A62</f>
         <v>Mg for eclampsia</v>
@@ -20707,8 +20812,9 @@
       <c r="B63" s="122" t="s">
         <v>272</v>
       </c>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="C63" s="34"/>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A64" t="str">
         <f>'Programs to include'!A33</f>
         <v>Mg for pre-eclampsia</v>
@@ -20716,8 +20822,9 @@
       <c r="B64" s="122" t="s">
         <v>270</v>
       </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="C64" s="34"/>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A65" t="str">
         <f>A64</f>
         <v>Mg for pre-eclampsia</v>
@@ -20725,8 +20832,9 @@
       <c r="B65" s="122" t="s">
         <v>272</v>
       </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="C65" s="34"/>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A66" t="str">
         <f>'Programs to include'!A34</f>
         <v>Multiple micronutrient supplementation</v>
@@ -20734,8 +20842,9 @@
       <c r="B66" s="122" t="s">
         <v>270</v>
       </c>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="C66" s="34"/>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A67" t="str">
         <f>A66</f>
         <v>Multiple micronutrient supplementation</v>
@@ -20743,8 +20852,9 @@
       <c r="B67" s="122" t="s">
         <v>272</v>
       </c>
-    </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="C67" s="34"/>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A68" t="str">
         <f>'Programs to include'!A35</f>
         <v>Multiple micronutrient supplementation (malaria area)</v>
@@ -20752,8 +20862,9 @@
       <c r="B68" s="122" t="s">
         <v>270</v>
       </c>
-    </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="C68" s="34"/>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A69" t="str">
         <f>A68</f>
         <v>Multiple micronutrient supplementation (malaria area)</v>
@@ -20761,8 +20872,9 @@
       <c r="B69" s="122" t="s">
         <v>272</v>
       </c>
-    </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="C69" s="34"/>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A70" t="str">
         <f>'Programs to include'!A36</f>
         <v>Oral rehydration salts</v>
@@ -20770,8 +20882,9 @@
       <c r="B70" s="122" t="s">
         <v>270</v>
       </c>
-    </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="C70" s="34"/>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A71" t="str">
         <f>A70</f>
         <v>Oral rehydration salts</v>
@@ -20779,8 +20892,9 @@
       <c r="B71" s="122" t="s">
         <v>272</v>
       </c>
-    </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="C71" s="34"/>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A72" t="str">
         <f>'Programs to include'!A37</f>
         <v>Public provision of complementary foods</v>
@@ -20788,8 +20902,9 @@
       <c r="B72" s="122" t="s">
         <v>270</v>
       </c>
-    </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="C72" s="34"/>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A73" t="str">
         <f>A72</f>
         <v>Public provision of complementary foods</v>
@@ -20797,8 +20912,12 @@
       <c r="B73" s="122" t="s">
         <v>272</v>
       </c>
-    </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="C73" s="34"/>
+      <c r="D73">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A74" t="str">
         <f>'Programs to include'!A38</f>
         <v>Public provision of complementary foods with iron</v>
@@ -20806,8 +20925,9 @@
       <c r="B74" s="122" t="s">
         <v>270</v>
       </c>
-    </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="C74" s="34"/>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A75" t="str">
         <f>A74</f>
         <v>Public provision of complementary foods with iron</v>
@@ -20815,8 +20935,12 @@
       <c r="B75" s="122" t="s">
         <v>272</v>
       </c>
-    </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="C75" s="34"/>
+      <c r="D75">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A76" t="str">
         <f>'Programs to include'!A39</f>
         <v>Public provision of complementary foods with iron (malaria area)</v>
@@ -20824,8 +20948,9 @@
       <c r="B76" s="122" t="s">
         <v>270</v>
       </c>
-    </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="C76" s="34"/>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A77" t="str">
         <f>A76</f>
         <v>Public provision of complementary foods with iron (malaria area)</v>
@@ -20833,8 +20958,9 @@
       <c r="B77" s="122" t="s">
         <v>272</v>
       </c>
-    </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="C77" s="34"/>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A78" t="str">
         <f>'Programs to include'!A40</f>
         <v>Sprinkles</v>
@@ -20842,8 +20968,9 @@
       <c r="B78" s="122" t="s">
         <v>270</v>
       </c>
-    </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="C78" s="34"/>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A79" t="str">
         <f>A78</f>
         <v>Sprinkles</v>
@@ -20851,8 +20978,12 @@
       <c r="B79" s="122" t="s">
         <v>272</v>
       </c>
-    </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="C79" s="34"/>
+      <c r="D79">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A80" t="str">
         <f>'Programs to include'!A41</f>
         <v>Sprinkles (malaria area)</v>
@@ -20860,8 +20991,9 @@
       <c r="B80" s="122" t="s">
         <v>270</v>
       </c>
-    </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="C80" s="34"/>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A81" t="str">
         <f>A80</f>
         <v>Sprinkles (malaria area)</v>
@@ -20869,8 +21001,12 @@
       <c r="B81" s="122" t="s">
         <v>272</v>
       </c>
-    </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="C81" s="34"/>
+      <c r="D81">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A82" t="str">
         <f>'Programs to include'!A42</f>
         <v>Treatment of MAM</v>
@@ -20878,8 +21014,9 @@
       <c r="B82" s="122" t="s">
         <v>270</v>
       </c>
-    </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="C82" s="34"/>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A83" t="str">
         <f>A82</f>
         <v>Treatment of MAM</v>
@@ -20887,8 +21024,12 @@
       <c r="B83" s="122" t="s">
         <v>272</v>
       </c>
-    </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="C83" s="34"/>
+      <c r="D83">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A84" t="str">
         <f>'Programs to include'!A43</f>
         <v>Treatment of SAM</v>
@@ -20896,8 +21037,9 @@
       <c r="B84" s="122" t="s">
         <v>270</v>
       </c>
-    </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="C84" s="34"/>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A85" t="str">
         <f>A84</f>
         <v>Treatment of SAM</v>
@@ -20905,8 +21047,9 @@
       <c r="B85" s="122" t="s">
         <v>272</v>
       </c>
-    </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="C85" s="34"/>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A86" t="str">
         <f>'Programs to include'!A44</f>
         <v>Vitamin A supplementation</v>
@@ -20914,8 +21057,9 @@
       <c r="B86" s="122" t="s">
         <v>270</v>
       </c>
-    </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="C86" s="34"/>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A87" t="str">
         <f>A86</f>
         <v>Vitamin A supplementation</v>
@@ -20923,8 +21067,12 @@
       <c r="B87" s="122" t="s">
         <v>272</v>
       </c>
-    </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="C87" s="34"/>
+      <c r="D87">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A88" t="str">
         <f>'Programs to include'!A45</f>
         <v>WASH: Handwashing</v>
@@ -20932,8 +21080,9 @@
       <c r="B88" s="122" t="s">
         <v>270</v>
       </c>
-    </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="C88" s="34"/>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A89" t="str">
         <f>A88</f>
         <v>WASH: Handwashing</v>
@@ -20941,8 +21090,9 @@
       <c r="B89" s="122" t="s">
         <v>272</v>
       </c>
-    </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="C89" s="34"/>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A90" t="str">
         <f>'Programs to include'!A46</f>
         <v>WASH: Hygenic disposal</v>
@@ -20950,8 +21100,9 @@
       <c r="B90" s="122" t="s">
         <v>270</v>
       </c>
-    </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="C90" s="34"/>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A91" t="str">
         <f>A90</f>
         <v>WASH: Hygenic disposal</v>
@@ -20959,8 +21110,9 @@
       <c r="B91" s="122" t="s">
         <v>272</v>
       </c>
-    </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="C91" s="34"/>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A92" t="str">
         <f>'Programs to include'!A47</f>
         <v>WASH: Improved sanitation</v>
@@ -20968,8 +21120,9 @@
       <c r="B92" s="122" t="s">
         <v>270</v>
       </c>
-    </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="C92" s="34"/>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A93" t="str">
         <f>A92</f>
         <v>WASH: Improved sanitation</v>
@@ -20977,8 +21130,9 @@
       <c r="B93" s="122" t="s">
         <v>272</v>
       </c>
-    </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="C93" s="34"/>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A94" t="str">
         <f>'Programs to include'!A48</f>
         <v>WASH: Improved water source</v>
@@ -20986,8 +21140,9 @@
       <c r="B94" s="122" t="s">
         <v>270</v>
       </c>
-    </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="C94" s="34"/>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A95" t="str">
         <f>A94</f>
         <v>WASH: Improved water source</v>
@@ -20995,8 +21150,9 @@
       <c r="B95" s="122" t="s">
         <v>272</v>
       </c>
-    </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="C95" s="34"/>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A96" t="str">
         <f>'Programs to include'!A49</f>
         <v>WASH: Piped water</v>
@@ -21004,8 +21160,9 @@
       <c r="B96" s="122" t="s">
         <v>270</v>
       </c>
-    </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="C96" s="34"/>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A97" t="str">
         <f>A96</f>
         <v>WASH: Piped water</v>
@@ -21013,8 +21170,9 @@
       <c r="B97" s="122" t="s">
         <v>272</v>
       </c>
-    </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="C97" s="34"/>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A98" t="str">
         <f>'Programs to include'!A50</f>
         <v>Zinc for treatment + ORS</v>
@@ -21022,8 +21180,9 @@
       <c r="B98" s="122" t="s">
         <v>270</v>
       </c>
-    </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="C98" s="34"/>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A99" t="str">
         <f>A98</f>
         <v>Zinc for treatment + ORS</v>
@@ -21031,8 +21190,9 @@
       <c r="B99" s="122" t="s">
         <v>272</v>
       </c>
-    </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="C99" s="34"/>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A100" t="str">
         <f>'Programs to include'!A51</f>
         <v>Zinc supplementation</v>
@@ -21040,8 +21200,9 @@
       <c r="B100" s="122" t="s">
         <v>270</v>
       </c>
-    </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="C100" s="34"/>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A101" t="str">
         <f>A100</f>
         <v>Zinc supplementation</v>
@@ -21049,8 +21210,9 @@
       <c r="B101" s="122" t="s">
         <v>272</v>
       </c>
-    </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="C101" s="34"/>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A102" t="str">
         <f>'Programs to include'!A52</f>
         <v>IYCF 1</v>
@@ -21058,8 +21220,9 @@
       <c r="B102" s="122" t="s">
         <v>270</v>
       </c>
-    </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="C102" s="34"/>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A103" t="str">
         <f>A102</f>
         <v>IYCF 1</v>
@@ -21067,8 +21230,12 @@
       <c r="B103" s="122" t="s">
         <v>272</v>
       </c>
-    </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="C103" s="34"/>
+      <c r="D103">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A104" t="str">
         <f>'Programs to include'!A53</f>
         <v>IYCF 2</v>
@@ -21076,8 +21243,9 @@
       <c r="B104" s="122" t="s">
         <v>270</v>
       </c>
-    </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="C104" s="34"/>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A105" t="str">
         <f>A104</f>
         <v>IYCF 2</v>
@@ -21085,8 +21253,9 @@
       <c r="B105" s="122" t="s">
         <v>272</v>
       </c>
-    </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="C105" s="34"/>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A106" t="str">
         <f>'Programs to include'!A54</f>
         <v>IYCF 3</v>
@@ -21094,8 +21263,9 @@
       <c r="B106" s="122" t="s">
         <v>270</v>
       </c>
-    </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="C106" s="34"/>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A107" t="str">
         <f>A106</f>
         <v>IYCF 3</v>
@@ -21103,9 +21273,11 @@
       <c r="B107" s="122" t="s">
         <v>272</v>
       </c>
+      <c r="C107" s="34"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -21113,8 +21285,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1A00-000000000000}">
   <dimension ref="A1:E54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="B44" sqref="B44"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A44" sqref="A44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -21796,7 +21968,7 @@
         <v>Vitamin A supplementation</v>
       </c>
       <c r="B44" s="13">
-        <v>0.8</v>
+        <v>0</v>
       </c>
       <c r="C44" s="13">
         <v>0.95</v>
@@ -22957,8 +23129,8 @@
   </sheetPr>
   <dimension ref="A1:B54"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="B48" sqref="B48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -22979,209 +23151,157 @@
       <c r="A2" s="122" t="s">
         <v>55</v>
       </c>
-      <c r="B2" s="122" t="s">
-        <v>165</v>
-      </c>
+      <c r="B2" s="122"/>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A3" s="124" t="s">
         <v>266</v>
       </c>
-      <c r="B3" s="122" t="s">
-        <v>165</v>
-      </c>
+      <c r="B3" s="122"/>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A4" s="4" t="s">
         <v>263</v>
       </c>
-      <c r="B4" s="122" t="s">
-        <v>165</v>
-      </c>
+      <c r="B4" s="122"/>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A5" s="4" t="s">
         <v>143</v>
       </c>
-      <c r="B5" s="122" t="s">
-        <v>165</v>
-      </c>
+      <c r="B5" s="122"/>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A6" s="122" t="s">
         <v>185</v>
       </c>
-      <c r="B6" s="122" t="s">
-        <v>165</v>
-      </c>
+      <c r="B6" s="122"/>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A7" s="11" t="s">
         <v>145</v>
       </c>
-      <c r="B7" s="122" t="s">
-        <v>165</v>
-      </c>
+      <c r="B7" s="122"/>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A8" s="11" t="s">
         <v>146</v>
       </c>
-      <c r="B8" s="122" t="s">
-        <v>165</v>
-      </c>
+      <c r="B8" s="122"/>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A9" s="11" t="s">
         <v>144</v>
       </c>
-      <c r="B9" s="122" t="s">
-        <v>165</v>
-      </c>
+      <c r="B9" s="122"/>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A10" s="122" t="s">
         <v>124</v>
       </c>
-      <c r="B10" s="122" t="s">
-        <v>165</v>
-      </c>
+      <c r="B10" s="122"/>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A11" s="122" t="s">
         <v>132</v>
       </c>
-      <c r="B11" s="122" t="s">
-        <v>165</v>
-      </c>
+      <c r="B11" s="122"/>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A12" s="122" t="s">
         <v>125</v>
       </c>
-      <c r="B12" s="122" t="s">
-        <v>165</v>
-      </c>
+      <c r="B12" s="122"/>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A13" s="122" t="s">
         <v>133</v>
       </c>
-      <c r="B13" s="122" t="s">
-        <v>165</v>
-      </c>
+      <c r="B13" s="122"/>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A14" s="122" t="s">
         <v>126</v>
       </c>
-      <c r="B14" s="122" t="s">
-        <v>165</v>
-      </c>
+      <c r="B14" s="122"/>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A15" s="122" t="s">
         <v>134</v>
       </c>
-      <c r="B15" s="122" t="s">
-        <v>165</v>
-      </c>
+      <c r="B15" s="122"/>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A16" s="122" t="s">
         <v>123</v>
       </c>
-      <c r="B16" s="122" t="s">
-        <v>165</v>
-      </c>
+      <c r="B16" s="122"/>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A17" s="122" t="s">
         <v>131</v>
       </c>
-      <c r="B17" s="122" t="s">
-        <v>165</v>
-      </c>
+      <c r="B17" s="122"/>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A18" s="122" t="s">
         <v>121</v>
       </c>
-      <c r="B18" s="122" t="s">
-        <v>165</v>
-      </c>
+      <c r="B18" s="122"/>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A19" s="122" t="s">
         <v>129</v>
       </c>
-      <c r="B19" s="122" t="s">
-        <v>165</v>
-      </c>
+      <c r="B19" s="122"/>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A20" s="122" t="s">
         <v>122</v>
       </c>
-      <c r="B20" s="122" t="s">
-        <v>165</v>
-      </c>
+      <c r="B20" s="122"/>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A21" s="122" t="s">
         <v>130</v>
       </c>
-      <c r="B21" s="122" t="s">
-        <v>165</v>
-      </c>
+      <c r="B21" s="122"/>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A22" s="122" t="s">
         <v>120</v>
       </c>
-      <c r="B22" s="122" t="s">
-        <v>165</v>
-      </c>
+      <c r="B22" s="122"/>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A23" s="122" t="s">
         <v>128</v>
       </c>
-      <c r="B23" s="122" t="s">
-        <v>165</v>
-      </c>
+      <c r="B23" s="122"/>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A24" s="122" t="s">
         <v>119</v>
       </c>
-      <c r="B24" s="122" t="s">
-        <v>165</v>
-      </c>
+      <c r="B24" s="122"/>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A25" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="B25" s="122" t="s">
-        <v>165</v>
-      </c>
+      <c r="B25" s="122"/>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A26" s="4" t="s">
         <v>139</v>
       </c>
-      <c r="B26" s="122" t="s">
-        <v>165</v>
-      </c>
+      <c r="B26" s="122"/>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A27" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="B27" s="122" t="s">
-        <v>165</v>
-      </c>
+      <c r="B27" s="122"/>
     </row>
     <row r="28" spans="1:2" s="10" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A28" s="116" t="s">
@@ -23205,49 +23325,37 @@
       <c r="A31" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="B31" s="122" t="s">
-        <v>165</v>
-      </c>
+      <c r="B31" s="122"/>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A32" s="4" t="s">
         <v>265</v>
       </c>
-      <c r="B32" s="122" t="s">
-        <v>165</v>
-      </c>
+      <c r="B32" s="122"/>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A33" s="4" t="s">
         <v>264</v>
       </c>
-      <c r="B33" s="122" t="s">
-        <v>165</v>
-      </c>
+      <c r="B33" s="122"/>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A34" s="122" t="s">
         <v>135</v>
       </c>
-      <c r="B34" s="122" t="s">
-        <v>165</v>
-      </c>
+      <c r="B34" s="122"/>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A35" s="122" t="s">
         <v>138</v>
       </c>
-      <c r="B35" s="122" t="s">
-        <v>165</v>
-      </c>
+      <c r="B35" s="122"/>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A36" s="122" t="s">
         <v>261</v>
       </c>
-      <c r="B36" s="122" t="s">
-        <v>165</v>
-      </c>
+      <c r="B36" s="122"/>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A37" s="4" t="s">
@@ -23269,121 +23377,91 @@
       <c r="A39" s="4" t="s">
         <v>136</v>
       </c>
-      <c r="B39" s="122" t="s">
-        <v>165</v>
-      </c>
+      <c r="B39" s="122"/>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A40" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="B40" s="122" t="s">
-        <v>165</v>
-      </c>
+      <c r="B40" s="122"/>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A41" s="29" t="s">
         <v>137</v>
       </c>
-      <c r="B41" s="122" t="s">
-        <v>165</v>
-      </c>
+      <c r="B41" s="122"/>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A42" s="4" t="s">
         <v>151</v>
       </c>
-      <c r="B42" s="122" t="s">
-        <v>165</v>
-      </c>
+      <c r="B42" s="122"/>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A43" s="4" t="s">
         <v>152</v>
       </c>
-      <c r="B43" s="122" t="s">
-        <v>165</v>
-      </c>
+      <c r="B43" s="122"/>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A44" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="B44" s="122" t="s">
-        <v>165</v>
-      </c>
+      <c r="B44" s="122"/>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A45" s="122" t="s">
         <v>260</v>
       </c>
-      <c r="B45" s="122" t="s">
-        <v>165</v>
-      </c>
+      <c r="B45" s="122"/>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A46" s="122" t="s">
         <v>259</v>
       </c>
-      <c r="B46" s="122" t="s">
-        <v>165</v>
-      </c>
+      <c r="B46" s="122"/>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A47" s="122" t="s">
         <v>258</v>
       </c>
-      <c r="B47" s="122" t="s">
-        <v>165</v>
-      </c>
+      <c r="B47" s="122"/>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A48" s="122" t="s">
         <v>256</v>
       </c>
-      <c r="B48" s="122" t="s">
-        <v>165</v>
-      </c>
+      <c r="B48" s="122"/>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A49" s="122" t="s">
         <v>257</v>
       </c>
-      <c r="B49" s="122" t="s">
-        <v>165</v>
-      </c>
+      <c r="B49" s="122"/>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A50" s="122" t="s">
         <v>262</v>
       </c>
-      <c r="B50" s="122" t="s">
-        <v>165</v>
-      </c>
+      <c r="B50" s="122"/>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A51" s="4" t="s">
         <v>140</v>
       </c>
-      <c r="B51" s="122" t="s">
-        <v>165</v>
-      </c>
+      <c r="B51" s="122"/>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A52" s="125" t="s">
         <v>161</v>
       </c>
-      <c r="B52" s="122" t="s">
-        <v>165</v>
-      </c>
+      <c r="B52" s="122"/>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A53" s="125" t="s">
         <v>162</v>
       </c>
-      <c r="B53" s="122" t="s">
-        <v>165</v>
-      </c>
+      <c r="B53" s="122"/>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A54" s="125" t="s">

</xml_diff>

<commit_message>
Changed script import to get speed boost
</commit_message>
<xml_diff>
--- a/input_spreadsheets/Master/InputForCode_Master.xlsx
+++ b/input_spreadsheets/Master/InputForCode_Master.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10116"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10210"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="3460" yWindow="-21140" windowWidth="33240" windowHeight="21120" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-36140" yWindow="-21140" windowWidth="33240" windowHeight="21120" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Baseline year demographics" sheetId="1" r:id="rId1"/>
@@ -2612,7 +2612,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1273" uniqueCount="273">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1278" uniqueCount="273">
   <si>
     <t>year</t>
   </si>
@@ -6919,7 +6919,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
@@ -12910,11 +12910,6 @@
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="B36:B38"/>
-    <mergeCell ref="B39:B41"/>
-    <mergeCell ref="B42:B44"/>
-    <mergeCell ref="B45:B47"/>
-    <mergeCell ref="B48:B50"/>
     <mergeCell ref="B25:B27"/>
     <mergeCell ref="B28:B30"/>
     <mergeCell ref="B31:B33"/>
@@ -12925,6 +12920,11 @@
     <mergeCell ref="B14:B16"/>
     <mergeCell ref="B19:B21"/>
     <mergeCell ref="B22:B24"/>
+    <mergeCell ref="B36:B38"/>
+    <mergeCell ref="B39:B41"/>
+    <mergeCell ref="B42:B44"/>
+    <mergeCell ref="B45:B47"/>
+    <mergeCell ref="B48:B50"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -25400,10 +25400,13 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0EC07D7C-27C3-0245-A9EE-CC3E398BBA0F}">
-  <dimension ref="A1:K28"/>
+  <sheetPr>
+    <tabColor theme="7" tint="-0.249977111117893"/>
+  </sheetPr>
+  <dimension ref="A1:K32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L5" sqref="L5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K28" sqref="K28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -25827,6 +25830,29 @@
     <row r="28" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A28" s="9" t="s">
         <v>36</v>
+      </c>
+      <c r="B28" s="9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="B29" s="9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="B30" s="9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="B31" s="9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="B32" s="9" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -27114,7 +27140,7 @@
   <dimension ref="A1:J28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:F1"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -28857,7 +28883,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:C15"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Deleted few test values
</commit_message>
<xml_diff>
--- a/input_spreadsheets/Master/InputForCode_Master.xlsx
+++ b/input_spreadsheets/Master/InputForCode_Master.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-36140" yWindow="-21140" windowWidth="33240" windowHeight="21120" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-38340" yWindow="-21140" windowWidth="33240" windowHeight="21120" tabRatio="500" firstSheet="8" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Baseline year demographics" sheetId="1" r:id="rId1"/>
@@ -421,49 +421,6 @@
     <author>Sam</author>
   </authors>
   <commentList>
-    <comment ref="A19" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0A00-000001000000}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t>Sam:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t>We currently do not have data for correct appropriate comp feeding practices (cf BF practices), so this does nothing.</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
-<file path=xl/comments11.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
-  <authors>
-    <author>Sam</author>
-  </authors>
-  <commentList>
     <comment ref="E1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0B00-000001000000}">
       <text>
         <r>
@@ -511,7 +468,7 @@
 </comments>
 </file>
 
-<file path=xl/comments12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments11.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Sam</author>
@@ -593,7 +550,7 @@
 </comments>
 </file>
 
-<file path=xl/comments13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments12.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author xml:space="preserve"> Janka Petravic</author>
@@ -627,7 +584,7 @@
 </comments>
 </file>
 
-<file path=xl/comments14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments13.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author xml:space="preserve"> Janka Petravic</author>
@@ -1224,7 +1181,7 @@
 </comments>
 </file>
 
-<file path=xl/comments15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments14.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Sam</author>
@@ -1355,7 +1312,7 @@
 </comments>
 </file>
 
-<file path=xl/comments16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments15.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Ruth</author>
@@ -1389,7 +1346,7 @@
 </comments>
 </file>
 
-<file path=xl/comments17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments16.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author xml:space="preserve"> Janka Petravic</author>
@@ -1450,7 +1407,7 @@
 </comments>
 </file>
 
-<file path=xl/comments18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments17.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Sam</author>
@@ -1631,7 +1588,7 @@
 </comments>
 </file>
 
-<file path=xl/comments19.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments18.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Sam</author>
@@ -1682,6 +1639,49 @@
           </rPr>
           <t xml:space="preserve">
 When one program cannot exceed cov of another</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments19.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Sam</author>
+  </authors>
+  <commentList>
+    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{45B4E5D3-C5DC-6B43-822A-DF0A04E4F811}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Sam:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Constrains the coverage % scale-up from baseline</t>
         </r>
       </text>
     </comment>
@@ -1772,49 +1772,6 @@
 </file>
 
 <file path=xl/comments20.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
-  <authors>
-    <author>Sam</author>
-  </authors>
-  <commentList>
-    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{45B4E5D3-C5DC-6B43-822A-DF0A04E4F811}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Sam:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Constrains the coverage % scale-up from baseline</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
-<file path=xl/comments21.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Sam</author>
@@ -2317,40 +2274,6 @@
     <author>Sam</author>
   </authors>
   <commentList>
-    <comment ref="A46" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0800-000001000000}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t>Sam:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Not modelling death through anaemia</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
-<file path=xl/comments9.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
-  <authors>
-    <author>Sam</author>
-  </authors>
-  <commentList>
     <comment ref="A6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0900-000001000000}">
       <text>
         <r>
@@ -2604,6 +2527,49 @@
           </rPr>
           <t xml:space="preserve">
 Fictional</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments9.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Sam</author>
+  </authors>
+  <commentList>
+    <comment ref="A19" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0A00-000001000000}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Sam:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>We currently do not have data for correct appropriate comp feeding practices (cf BF practices), so this does nothing.</t>
         </r>
       </text>
     </comment>
@@ -7356,14 +7322,14 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
   <dimension ref="A1:P100"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
+    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="C48" sqref="C48:C49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -11408,7 +11374,6 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -11420,7 +11385,7 @@
   <dimension ref="A1:G22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+      <selection activeCell="C13" sqref="C13:G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -17341,7 +17306,7 @@
   </sheetPr>
   <dimension ref="A1:H7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView zoomScale="137" zoomScaleNormal="137" workbookViewId="0">
       <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
@@ -23433,7 +23398,7 @@
   <dimension ref="A1:K14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F38" sqref="F38:F39"/>
+      <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -23511,7 +23476,7 @@
       <c r="H2" t="s">
         <v>164</v>
       </c>
-      <c r="J2" s="45" t="s">
+      <c r="J2" s="10" t="s">
         <v>164</v>
       </c>
     </row>
@@ -23540,7 +23505,7 @@
       <c r="H3" t="s">
         <v>164</v>
       </c>
-      <c r="J3" s="45" t="s">
+      <c r="J3" s="10" t="s">
         <v>164</v>
       </c>
     </row>
@@ -23569,7 +23534,7 @@
       <c r="H4" t="s">
         <v>164</v>
       </c>
-      <c r="J4" s="45" t="s">
+      <c r="J4" s="10" t="s">
         <v>164</v>
       </c>
     </row>
@@ -23598,7 +23563,7 @@
       <c r="H5" t="s">
         <v>164</v>
       </c>
-      <c r="J5" s="45" t="s">
+      <c r="J5" s="10" t="s">
         <v>164</v>
       </c>
     </row>
@@ -23627,7 +23592,7 @@
       <c r="H6" t="s">
         <v>164</v>
       </c>
-      <c r="J6" s="45" t="s">
+      <c r="J6" s="10" t="s">
         <v>164</v>
       </c>
     </row>
@@ -23641,7 +23606,7 @@
       <c r="I7" t="s">
         <v>164</v>
       </c>
-      <c r="J7" s="45"/>
+      <c r="J7" s="10"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A8" s="9" t="s">
@@ -23653,7 +23618,7 @@
       <c r="I8" t="s">
         <v>164</v>
       </c>
-      <c r="J8" s="45"/>
+      <c r="J8" s="10"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A9" s="9" t="s">
@@ -23665,7 +23630,7 @@
       <c r="I9" t="s">
         <v>164</v>
       </c>
-      <c r="J9" s="45"/>
+      <c r="J9" s="10"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A10" s="9" t="s">
@@ -23677,7 +23642,7 @@
       <c r="I10" t="s">
         <v>164</v>
       </c>
-      <c r="J10" s="45"/>
+      <c r="J10" s="10"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A11" s="9" t="s">
@@ -24225,8 +24190,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD451538-A103-E449-A7A9-980845064FD1}">
   <dimension ref="A1:Y107"/>
   <sheetViews>
-    <sheetView topLeftCell="A63" workbookViewId="0">
-      <selection activeCell="D77" sqref="A1:XFD1048576"/>
+    <sheetView topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="D103" sqref="D103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -24938,7 +24903,7 @@
       </c>
       <c r="C64" s="34"/>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A65" t="str">
         <f>A64</f>
         <v>Mg for pre-eclampsia</v>
@@ -24948,7 +24913,7 @@
       </c>
       <c r="C65" s="34"/>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A66" t="str">
         <f>'Programs to include'!A34</f>
         <v>Multiple micronutrient supplementation</v>
@@ -24958,7 +24923,7 @@
       </c>
       <c r="C66" s="34"/>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A67" t="str">
         <f>A66</f>
         <v>Multiple micronutrient supplementation</v>
@@ -24968,7 +24933,7 @@
       </c>
       <c r="C67" s="34"/>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A68" t="str">
         <f>'Programs to include'!A35</f>
         <v>Multiple micronutrient supplementation (malaria area)</v>
@@ -24978,7 +24943,7 @@
       </c>
       <c r="C68" s="34"/>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A69" t="str">
         <f>A68</f>
         <v>Multiple micronutrient supplementation (malaria area)</v>
@@ -24988,7 +24953,7 @@
       </c>
       <c r="C69" s="34"/>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A70" t="str">
         <f>'Programs to include'!A36</f>
         <v>Oral rehydration salts</v>
@@ -24998,7 +24963,7 @@
       </c>
       <c r="C70" s="34"/>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A71" t="str">
         <f>A70</f>
         <v>Oral rehydration salts</v>
@@ -25008,7 +24973,7 @@
       </c>
       <c r="C71" s="34"/>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A72" t="str">
         <f>'Programs to include'!A37</f>
         <v>Public provision of complementary foods</v>
@@ -25018,7 +24983,7 @@
       </c>
       <c r="C72" s="34"/>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A73" t="str">
         <f>A72</f>
         <v>Public provision of complementary foods</v>
@@ -25027,11 +24992,8 @@
         <v>271</v>
       </c>
       <c r="C73" s="34"/>
-      <c r="D73">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.15">
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A74" t="str">
         <f>'Programs to include'!A38</f>
         <v>Public provision of complementary foods with iron</v>
@@ -25041,7 +25003,7 @@
       </c>
       <c r="C74" s="34"/>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A75" t="str">
         <f>A74</f>
         <v>Public provision of complementary foods with iron</v>
@@ -25050,11 +25012,8 @@
         <v>271</v>
       </c>
       <c r="C75" s="34"/>
-      <c r="D75">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.15">
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A76" t="str">
         <f>'Programs to include'!A39</f>
         <v>Public provision of complementary foods with iron (malaria area)</v>
@@ -25064,7 +25023,7 @@
       </c>
       <c r="C76" s="34"/>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A77" t="str">
         <f>A76</f>
         <v>Public provision of complementary foods with iron (malaria area)</v>
@@ -25073,11 +25032,8 @@
         <v>271</v>
       </c>
       <c r="C77" s="34"/>
-      <c r="D77">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.15">
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A78" t="str">
         <f>'Programs to include'!A40</f>
         <v>Sprinkles</v>
@@ -25087,7 +25043,7 @@
       </c>
       <c r="C78" s="34"/>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A79" t="str">
         <f>A78</f>
         <v>Sprinkles</v>
@@ -25096,11 +25052,8 @@
         <v>271</v>
       </c>
       <c r="C79" s="34"/>
-      <c r="D79">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.15">
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A80" t="str">
         <f>'Programs to include'!A41</f>
         <v>Sprinkles (malaria area)</v>
@@ -25110,7 +25063,7 @@
       </c>
       <c r="C80" s="34"/>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A81" t="str">
         <f>A80</f>
         <v>Sprinkles (malaria area)</v>
@@ -25119,11 +25072,8 @@
         <v>271</v>
       </c>
       <c r="C81" s="34"/>
-      <c r="D81">
-        <v>0.95</v>
-      </c>
-    </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.15">
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A82" t="str">
         <f>'Programs to include'!A42</f>
         <v>Treatment of MAM</v>
@@ -25133,7 +25083,7 @@
       </c>
       <c r="C82" s="34"/>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A83" t="str">
         <f>A82</f>
         <v>Treatment of MAM</v>
@@ -25142,11 +25092,8 @@
         <v>271</v>
       </c>
       <c r="C83" s="34"/>
-      <c r="D83">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.15">
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A84" t="str">
         <f>'Programs to include'!A43</f>
         <v>Treatment of SAM</v>
@@ -25156,7 +25103,7 @@
       </c>
       <c r="C84" s="34"/>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A85" t="str">
         <f>A84</f>
         <v>Treatment of SAM</v>
@@ -25166,7 +25113,7 @@
       </c>
       <c r="C85" s="34"/>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A86" t="str">
         <f>'Programs to include'!A44</f>
         <v>Vitamin A supplementation</v>
@@ -25176,7 +25123,7 @@
       </c>
       <c r="C86" s="34"/>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A87" t="str">
         <f>A86</f>
         <v>Vitamin A supplementation</v>
@@ -25185,11 +25132,8 @@
         <v>271</v>
       </c>
       <c r="C87" s="34"/>
-      <c r="D87">
-        <v>0.95</v>
-      </c>
-    </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.15">
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A88" t="str">
         <f>'Programs to include'!A45</f>
         <v>WASH: Handwashing</v>
@@ -25199,7 +25143,7 @@
       </c>
       <c r="C88" s="34"/>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A89" t="str">
         <f>A88</f>
         <v>WASH: Handwashing</v>
@@ -25209,7 +25153,7 @@
       </c>
       <c r="C89" s="34"/>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A90" t="str">
         <f>'Programs to include'!A46</f>
         <v>WASH: Hygenic disposal</v>
@@ -25219,7 +25163,7 @@
       </c>
       <c r="C90" s="34"/>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A91" t="str">
         <f>A90</f>
         <v>WASH: Hygenic disposal</v>
@@ -25229,7 +25173,7 @@
       </c>
       <c r="C91" s="34"/>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A92" t="str">
         <f>'Programs to include'!A47</f>
         <v>WASH: Improved sanitation</v>
@@ -25239,7 +25183,7 @@
       </c>
       <c r="C92" s="34"/>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="93" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A93" t="str">
         <f>A92</f>
         <v>WASH: Improved sanitation</v>
@@ -25249,7 +25193,7 @@
       </c>
       <c r="C93" s="34"/>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A94" t="str">
         <f>'Programs to include'!A48</f>
         <v>WASH: Improved water source</v>
@@ -25259,7 +25203,7 @@
       </c>
       <c r="C94" s="34"/>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="95" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A95" t="str">
         <f>A94</f>
         <v>WASH: Improved water source</v>
@@ -25269,7 +25213,7 @@
       </c>
       <c r="C95" s="34"/>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="96" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A96" t="str">
         <f>'Programs to include'!A49</f>
         <v>WASH: Piped water</v>
@@ -25279,7 +25223,7 @@
       </c>
       <c r="C96" s="34"/>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A97" t="str">
         <f>A96</f>
         <v>WASH: Piped water</v>
@@ -25289,7 +25233,7 @@
       </c>
       <c r="C97" s="34"/>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="98" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A98" t="str">
         <f>'Programs to include'!A50</f>
         <v>Zinc for treatment + ORS</v>
@@ -25299,7 +25243,7 @@
       </c>
       <c r="C98" s="34"/>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="99" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A99" t="str">
         <f>A98</f>
         <v>Zinc for treatment + ORS</v>
@@ -25309,7 +25253,7 @@
       </c>
       <c r="C99" s="34"/>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="100" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A100" t="str">
         <f>'Programs to include'!A51</f>
         <v>Zinc supplementation</v>
@@ -25319,7 +25263,7 @@
       </c>
       <c r="C100" s="34"/>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="101" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A101" t="str">
         <f>A100</f>
         <v>Zinc supplementation</v>
@@ -25329,7 +25273,7 @@
       </c>
       <c r="C101" s="34"/>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="102" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A102" t="str">
         <f>'Programs to include'!A52</f>
         <v>IYCF 1</v>
@@ -25339,7 +25283,7 @@
       </c>
       <c r="C102" s="34"/>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="103" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A103" t="str">
         <f>A102</f>
         <v>IYCF 1</v>
@@ -25348,11 +25292,8 @@
         <v>271</v>
       </c>
       <c r="C103" s="34"/>
-      <c r="D103">
-        <v>0.95</v>
-      </c>
-    </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.15">
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A104" t="str">
         <f>'Programs to include'!A53</f>
         <v>IYCF 2</v>
@@ -25362,7 +25303,7 @@
       </c>
       <c r="C104" s="34"/>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="105" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A105" t="str">
         <f>A104</f>
         <v>IYCF 2</v>
@@ -25372,7 +25313,7 @@
       </c>
       <c r="C105" s="34"/>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="106" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A106" t="str">
         <f>'Programs to include'!A54</f>
         <v>IYCF 3</v>
@@ -25382,7 +25323,7 @@
       </c>
       <c r="C106" s="34"/>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="107" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A107" t="str">
         <f>A106</f>
         <v>IYCF 3</v>
@@ -25405,8 +25346,8 @@
   </sheetPr>
   <dimension ref="A1:K32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K28" sqref="K28"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -26787,8 +26728,8 @@
   </sheetPr>
   <dimension ref="A1:B54"/>
   <sheetViews>
-    <sheetView topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="B39" sqref="B39"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>

</xml_diff>

<commit_message>
Added mortality for PW
</commit_message>
<xml_diff>
--- a/input_spreadsheets/Master/InputForCode_Master.xlsx
+++ b/input_spreadsheets/Master/InputForCode_Master.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/samhainsworth/Desktop/Github Projects/Nutrition/input_spreadsheets/Master/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F54D6B26-C786-ED47-8CE2-E0793204EB09}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7758ADEE-5DCD-B14F-8C2E-E90D847232F0}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="800" yWindow="-21140" windowWidth="33240" windowHeight="21120" tabRatio="500" firstSheet="21" activeTab="25" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="800" yWindow="-21140" windowWidth="33240" windowHeight="21120" tabRatio="500" firstSheet="21" activeTab="26" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Baseline year demographics" sheetId="1" r:id="rId1"/>
@@ -2579,7 +2579,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1263" uniqueCount="270">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1267" uniqueCount="270">
   <si>
     <t>year</t>
   </si>
@@ -22613,7 +22613,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1800-000000000000}">
   <dimension ref="A1:K51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
@@ -23204,8 +23204,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1900-000000000000}">
   <dimension ref="A1:K14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7:H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -23410,6 +23410,9 @@
       <c r="C7" t="s">
         <v>161</v>
       </c>
+      <c r="H7" t="s">
+        <v>161</v>
+      </c>
       <c r="I7" t="s">
         <v>161</v>
       </c>
@@ -23422,6 +23425,9 @@
       <c r="C8" t="s">
         <v>161</v>
       </c>
+      <c r="H8" t="s">
+        <v>161</v>
+      </c>
       <c r="I8" t="s">
         <v>161</v>
       </c>
@@ -23434,6 +23440,9 @@
       <c r="C9" t="s">
         <v>161</v>
       </c>
+      <c r="H9" t="s">
+        <v>161</v>
+      </c>
       <c r="I9" t="s">
         <v>161</v>
       </c>
@@ -23444,6 +23453,9 @@
         <v>114</v>
       </c>
       <c r="C10" t="s">
+        <v>161</v>
+      </c>
+      <c r="H10" t="s">
         <v>161</v>
       </c>
       <c r="I10" t="s">

</xml_diff>

<commit_message>
Distinguishing between reference, fixed and current spending for optimisation
</commit_message>
<xml_diff>
--- a/input_spreadsheets/Master/InputForCode_Master.xlsx
+++ b/input_spreadsheets/Master/InputForCode_Master.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/samhainsworth/Desktop/Github Projects/Nutrition/input_spreadsheets/Master/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F5FBC65-ADA9-8E41-9D28-C5F4872EB2C3}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DF07826-4F18-C349-90C4-DD5C24F4146B}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="19180" windowHeight="15540" tabRatio="500" firstSheet="17" activeTab="17" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="12800" windowHeight="15540" tabRatio="500" firstSheet="17" activeTab="17" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Baseline year demographics" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
     <sheet name="Programs annual spending" sheetId="52" r:id="rId15"/>
     <sheet name="Reference programs" sheetId="48" r:id="rId16"/>
     <sheet name="Programs cost and coverage" sheetId="20" r:id="rId17"/>
-    <sheet name="Expenditure &amp; budget" sheetId="54" r:id="rId18"/>
+    <sheet name="Expenditure &amp; budget" sheetId="56" r:id="rId18"/>
     <sheet name="Appropriate breastfeeding" sheetId="19" r:id="rId19"/>
     <sheet name="IYCF package odds ratios" sheetId="32" r:id="rId20"/>
     <sheet name="Relative risks" sheetId="26" r:id="rId21"/>
@@ -4201,7 +4201,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="725">
+  <cellStyleXfs count="726">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -4927,8 +4927,9 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="139">
+  <cellXfs count="141">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -5163,9 +5164,11 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="725" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="11" fontId="5" fillId="0" borderId="0" xfId="725" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="725" applyFont="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="725">
+  <cellStyles count="726">
     <cellStyle name="Comma" xfId="9" builtinId="3"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
@@ -5890,6 +5893,7 @@
     <cellStyle name="Hyperlink" xfId="721" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="723" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="725" xr:uid="{4853C94F-AF78-4A40-8545-F3F2355BCD39}"/>
     <cellStyle name="Percent" xfId="10" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -11342,7 +11346,7 @@
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE56F303-2593-8C4B-B9BC-7E4885C4A876}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C89E6627-83D6-8847-A6C6-AF1834DAC255}">
   <sheetPr>
     <tabColor theme="7" tint="-0.249977111117893"/>
   </sheetPr>
@@ -11354,31 +11358,32 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="17.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.5" style="138" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.83203125" style="138" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="10.83203125" style="138"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="140" t="s">
         <v>264</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="140" t="s">
         <v>269</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="140" t="s">
         <v>267</v>
       </c>
-      <c r="B2" s="138">
+      <c r="B2" s="139">
         <v>1000000</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="140" t="s">
         <v>268</v>
       </c>
-      <c r="B3" s="138"/>
+      <c r="B3" s="139"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Scripts to get prevalences and scaled unit costs
</commit_message>
<xml_diff>
--- a/input_spreadsheets/Master/InputForCode_Master.xlsx
+++ b/input_spreadsheets/Master/InputForCode_Master.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/samhainsworth/Desktop/Github Projects/Nutrition/input_spreadsheets/Master/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02CA1CC1-F06B-304F-8B6D-3835EF4DAE19}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{098A2C2A-A51F-0C45-AD4D-D14873ED4E8D}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="12800" windowHeight="15540" tabRatio="500" firstSheet="16" activeTab="16" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="12800" windowHeight="15540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Baseline year demographics" sheetId="1" r:id="rId1"/>
@@ -64,7 +64,7 @@
     <definedName name="PWPop">'Baseline year demographics'!$C$44:$C$47</definedName>
     <definedName name="WRAPop">'Baseline year demographics'!$C$32:$C$35</definedName>
   </definedNames>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -146,7 +146,7 @@
           <rPr>
             <b/>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Arial"/>
             <family val="2"/>
           </rPr>
@@ -155,12 +155,21 @@
         <r>
           <rPr>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Arial"/>
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-Number of stillbirths per 1000 TOTAL births</t>
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t>Number of stillbirths per 1000 TOTAL births</t>
         </r>
       </text>
     </comment>
@@ -170,7 +179,7 @@
           <rPr>
             <b/>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Arial"/>
             <family val="2"/>
           </rPr>
@@ -179,12 +188,21 @@
         <r>
           <rPr>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Arial"/>
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-Per 1000 live births</t>
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t>Per 1000 live births</t>
         </r>
       </text>
     </comment>
@@ -3501,15 +3519,6 @@
     <t>maternal mortality</t>
   </si>
   <si>
-    <t>neonatal mortality</t>
-  </si>
-  <si>
-    <t>infant mortality</t>
-  </si>
-  <si>
-    <t>under 5 mortality</t>
-  </si>
-  <si>
     <t>OR stunting progression</t>
   </si>
   <si>
@@ -3763,6 +3772,15 @@
   </si>
   <si>
     <t>Value</t>
+  </si>
+  <si>
+    <t>neonatal</t>
+  </si>
+  <si>
+    <t>infant</t>
+  </si>
+  <si>
+    <t>under 5</t>
   </si>
 </sst>
 </file>
@@ -7316,8 +7334,8 @@
   </sheetPr>
   <dimension ref="A1:E56"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" zoomScale="125" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="125" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -7423,7 +7441,7 @@
     </row>
     <row r="12" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B12" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="C12" s="130">
         <v>0.9</v>
@@ -7431,7 +7449,7 @@
     </row>
     <row r="13" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B13" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="C13" s="130">
         <v>0.1</v>
@@ -7439,7 +7457,7 @@
     </row>
     <row r="14" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B14" s="4" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="C14" s="15">
         <v>0.2</v>
@@ -7482,24 +7500,24 @@
       </c>
     </row>
     <row r="20" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B20" t="s">
-        <v>182</v>
+      <c r="B20" s="98" t="s">
+        <v>267</v>
       </c>
       <c r="C20" s="15">
         <v>25.4</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B21" t="s">
-        <v>183</v>
+      <c r="B21" s="98" t="s">
+        <v>268</v>
       </c>
       <c r="C21" s="15">
         <v>34.68</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B22" t="s">
-        <v>184</v>
+      <c r="B22" s="98" t="s">
+        <v>269</v>
       </c>
       <c r="C22" s="15">
         <v>39.32</v>
@@ -7608,7 +7626,7 @@
     </row>
     <row r="38" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="7" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="B38" s="62" t="s">
         <v>104</v>
@@ -7662,7 +7680,7 @@
     </row>
     <row r="44" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="7" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="B44" s="62" t="s">
         <v>108</v>
@@ -8176,10 +8194,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.15">
@@ -8192,13 +8210,13 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A3" s="99" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="B3" s="98"/>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A4" s="4" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="B4" s="98"/>
     </row>
@@ -8348,13 +8366,13 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A29" s="4" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="B29" s="98"/>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A30" s="4" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="B30" s="98"/>
     </row>
@@ -8372,7 +8390,7 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A33" s="98" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="B33" s="98"/>
     </row>
@@ -8434,7 +8452,7 @@
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A42" s="98" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="B42" s="98" t="s">
         <v>158</v>
@@ -8442,7 +8460,7 @@
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A43" s="98" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="B43" s="98" t="s">
         <v>158</v>
@@ -8450,25 +8468,25 @@
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A44" s="98" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="B44" s="98"/>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A45" s="98" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="B45" s="98"/>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A46" s="98" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="B46" s="98"/>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A47" s="98" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="B47" s="98"/>
     </row>
@@ -8522,13 +8540,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A1" s="7" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.15">
@@ -8765,7 +8783,7 @@
         <v>Public provision of complementary foods</v>
       </c>
       <c r="B34" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.15">
@@ -8911,10 +8929,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A1" s="7" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.15">
@@ -9392,10 +9410,10 @@
   <sheetData>
     <row r="1" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A1" s="7" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="C1" s="72">
         <f>'Baseline year demographics'!$C2+1</f>
@@ -9469,7 +9487,7 @@
         <v>Balanced energy-protein supplementation</v>
       </c>
       <c r="B2" s="98" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="C2" s="25"/>
     </row>
@@ -9479,7 +9497,7 @@
         <v>Balanced energy-protein supplementation</v>
       </c>
       <c r="B3" s="98" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="C3" s="25"/>
     </row>
@@ -9489,7 +9507,7 @@
         <v>Birth age program</v>
       </c>
       <c r="B4" s="98" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="C4" s="25"/>
     </row>
@@ -9499,7 +9517,7 @@
         <v>Birth age program</v>
       </c>
       <c r="B5" s="98" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="C5" s="25"/>
     </row>
@@ -9509,7 +9527,7 @@
         <v>Calcium supplementation</v>
       </c>
       <c r="B6" s="98" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="C6" s="25"/>
     </row>
@@ -9519,7 +9537,7 @@
         <v>Calcium supplementation</v>
       </c>
       <c r="B7" s="98" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="C7" s="25"/>
     </row>
@@ -9529,7 +9547,7 @@
         <v>Cash transfers</v>
       </c>
       <c r="B8" s="98" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="C8" s="25"/>
     </row>
@@ -9539,7 +9557,7 @@
         <v>Cash transfers</v>
       </c>
       <c r="B9" s="98" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="C9" s="25"/>
     </row>
@@ -9549,7 +9567,7 @@
         <v>Family Planning</v>
       </c>
       <c r="B10" s="98" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="C10" s="25"/>
     </row>
@@ -9559,7 +9577,7 @@
         <v>Family Planning</v>
       </c>
       <c r="B11" s="98" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="C11" s="25"/>
     </row>
@@ -9569,7 +9587,7 @@
         <v>IFA fortification of maize</v>
       </c>
       <c r="B12" s="98" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="C12" s="25"/>
     </row>
@@ -9579,7 +9597,7 @@
         <v>IFA fortification of maize</v>
       </c>
       <c r="B13" s="98" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="C13" s="25"/>
     </row>
@@ -9589,7 +9607,7 @@
         <v>IFA fortification of rice</v>
       </c>
       <c r="B14" s="98" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="C14" s="25"/>
     </row>
@@ -9599,7 +9617,7 @@
         <v>IFA fortification of rice</v>
       </c>
       <c r="B15" s="98" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="C15" s="25"/>
     </row>
@@ -9609,7 +9627,7 @@
         <v>IFA fortification of wheat flour</v>
       </c>
       <c r="B16" s="98" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="C16" s="25"/>
     </row>
@@ -9619,7 +9637,7 @@
         <v>IFA fortification of wheat flour</v>
       </c>
       <c r="B17" s="98" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="C17" s="25"/>
     </row>
@@ -9629,7 +9647,7 @@
         <v>IFAS not poor: community</v>
       </c>
       <c r="B18" s="98" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="C18" s="25"/>
     </row>
@@ -9639,7 +9657,7 @@
         <v>IFAS not poor: community</v>
       </c>
       <c r="B19" s="98" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="C19" s="25"/>
     </row>
@@ -9649,7 +9667,7 @@
         <v>IFAS not poor: community (malaria area)</v>
       </c>
       <c r="B20" s="98" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="C20" s="25"/>
     </row>
@@ -9659,7 +9677,7 @@
         <v>IFAS not poor: community (malaria area)</v>
       </c>
       <c r="B21" s="98" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="C21" s="25"/>
     </row>
@@ -9669,7 +9687,7 @@
         <v>IFAS not poor: hospital</v>
       </c>
       <c r="B22" s="98" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="C22" s="25"/>
     </row>
@@ -9679,7 +9697,7 @@
         <v>IFAS not poor: hospital</v>
       </c>
       <c r="B23" s="98" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="C23" s="25"/>
     </row>
@@ -9689,7 +9707,7 @@
         <v>IFAS not poor: hospital (malaria area)</v>
       </c>
       <c r="B24" s="98" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="C24" s="25"/>
     </row>
@@ -9699,7 +9717,7 @@
         <v>IFAS not poor: hospital (malaria area)</v>
       </c>
       <c r="B25" s="98" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="C25" s="25"/>
     </row>
@@ -9709,7 +9727,7 @@
         <v>IFAS not poor: retailer</v>
       </c>
       <c r="B26" s="98" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="C26" s="25"/>
     </row>
@@ -9719,7 +9737,7 @@
         <v>IFAS not poor: retailer</v>
       </c>
       <c r="B27" s="98" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="C27" s="25"/>
     </row>
@@ -9729,7 +9747,7 @@
         <v>IFAS not poor: retailer (malaria area)</v>
       </c>
       <c r="B28" s="98" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="C28" s="25"/>
     </row>
@@ -9739,7 +9757,7 @@
         <v>IFAS not poor: retailer (malaria area)</v>
       </c>
       <c r="B29" s="98" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="C29" s="25"/>
     </row>
@@ -9749,7 +9767,7 @@
         <v>IFAS not poor: school</v>
       </c>
       <c r="B30" s="98" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="C30" s="25"/>
     </row>
@@ -9759,7 +9777,7 @@
         <v>IFAS not poor: school</v>
       </c>
       <c r="B31" s="98" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="C31" s="25"/>
     </row>
@@ -9769,7 +9787,7 @@
         <v>IFAS not poor: school (malaria area)</v>
       </c>
       <c r="B32" s="98" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="C32" s="25"/>
     </row>
@@ -9779,7 +9797,7 @@
         <v>IFAS not poor: school (malaria area)</v>
       </c>
       <c r="B33" s="98" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="C33" s="25"/>
     </row>
@@ -9789,7 +9807,7 @@
         <v>IFAS poor: community</v>
       </c>
       <c r="B34" s="98" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="C34" s="25"/>
     </row>
@@ -9799,7 +9817,7 @@
         <v>IFAS poor: community</v>
       </c>
       <c r="B35" s="98" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="C35" s="25"/>
     </row>
@@ -9809,7 +9827,7 @@
         <v>IFAS poor: community (malaria area)</v>
       </c>
       <c r="B36" s="98" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="C36" s="25"/>
     </row>
@@ -9819,7 +9837,7 @@
         <v>IFAS poor: community (malaria area)</v>
       </c>
       <c r="B37" s="98" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="C37" s="25"/>
     </row>
@@ -9829,7 +9847,7 @@
         <v>IFAS poor: hospital</v>
       </c>
       <c r="B38" s="98" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="C38" s="25"/>
     </row>
@@ -9839,7 +9857,7 @@
         <v>IFAS poor: hospital</v>
       </c>
       <c r="B39" s="98" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="C39" s="25"/>
     </row>
@@ -9849,7 +9867,7 @@
         <v>IFAS poor: hospital (malaria area)</v>
       </c>
       <c r="B40" s="98" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="C40" s="25"/>
     </row>
@@ -9859,7 +9877,7 @@
         <v>IFAS poor: hospital (malaria area)</v>
       </c>
       <c r="B41" s="98" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="C41" s="25"/>
     </row>
@@ -9869,7 +9887,7 @@
         <v>IFAS poor: school</v>
       </c>
       <c r="B42" s="98" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="C42" s="25"/>
     </row>
@@ -9879,7 +9897,7 @@
         <v>IFAS poor: school</v>
       </c>
       <c r="B43" s="98" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="C43" s="25"/>
     </row>
@@ -9889,7 +9907,7 @@
         <v>IFAS poor: school (malaria area)</v>
       </c>
       <c r="B44" s="98" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="C44" s="25"/>
     </row>
@@ -9899,7 +9917,7 @@
         <v>IFAS poor: school (malaria area)</v>
       </c>
       <c r="B45" s="98" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="C45" s="25"/>
     </row>
@@ -9909,7 +9927,7 @@
         <v>IPTp</v>
       </c>
       <c r="B46" s="98" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="C46" s="25"/>
     </row>
@@ -9919,7 +9937,7 @@
         <v>IPTp</v>
       </c>
       <c r="B47" s="98" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="C47" s="25"/>
     </row>
@@ -9929,7 +9947,7 @@
         <v>Iron and folic acid supplementation for pregnant women</v>
       </c>
       <c r="B48" s="98" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="C48" s="25"/>
     </row>
@@ -9939,7 +9957,7 @@
         <v>Iron and folic acid supplementation for pregnant women</v>
       </c>
       <c r="B49" s="98" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="C49" s="25"/>
     </row>
@@ -9949,7 +9967,7 @@
         <v>Iron and folic acid supplementation for pregnant women (malaria area)</v>
       </c>
       <c r="B50" s="98" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="C50" s="25"/>
     </row>
@@ -9959,7 +9977,7 @@
         <v>Iron and folic acid supplementation for pregnant women (malaria area)</v>
       </c>
       <c r="B51" s="98" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="C51" s="25"/>
     </row>
@@ -9969,7 +9987,7 @@
         <v>Iron and iodine fortification of salt</v>
       </c>
       <c r="B52" s="98" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="C52" s="25"/>
     </row>
@@ -9979,7 +9997,7 @@
         <v>Iron and iodine fortification of salt</v>
       </c>
       <c r="B53" s="98" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="C53" s="25"/>
     </row>
@@ -9989,7 +10007,7 @@
         <v>Long-lasting insecticide-treated bednets</v>
       </c>
       <c r="B54" s="98" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="C54" s="25"/>
     </row>
@@ -9999,7 +10017,7 @@
         <v>Long-lasting insecticide-treated bednets</v>
       </c>
       <c r="B55" s="98" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="C55" s="25"/>
     </row>
@@ -10009,7 +10027,7 @@
         <v>Mg for eclampsia</v>
       </c>
       <c r="B56" s="98" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="C56" s="25"/>
     </row>
@@ -10019,7 +10037,7 @@
         <v>Mg for eclampsia</v>
       </c>
       <c r="B57" s="98" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="C57" s="25"/>
     </row>
@@ -10029,7 +10047,7 @@
         <v>Mg for pre-eclampsia</v>
       </c>
       <c r="B58" s="98" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="C58" s="25"/>
     </row>
@@ -10039,7 +10057,7 @@
         <v>Mg for pre-eclampsia</v>
       </c>
       <c r="B59" s="98" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="C59" s="25"/>
     </row>
@@ -10049,7 +10067,7 @@
         <v>Multiple micronutrient supplementation</v>
       </c>
       <c r="B60" s="98" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="C60" s="25"/>
     </row>
@@ -10059,7 +10077,7 @@
         <v>Multiple micronutrient supplementation</v>
       </c>
       <c r="B61" s="98" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="C61" s="25"/>
     </row>
@@ -10069,7 +10087,7 @@
         <v>Multiple micronutrient supplementation (malaria area)</v>
       </c>
       <c r="B62" s="98" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="C62" s="25"/>
     </row>
@@ -10079,7 +10097,7 @@
         <v>Multiple micronutrient supplementation (malaria area)</v>
       </c>
       <c r="B63" s="98" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="C63" s="25"/>
     </row>
@@ -10089,7 +10107,7 @@
         <v>Oral rehydration salts</v>
       </c>
       <c r="B64" s="98" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="C64" s="25"/>
     </row>
@@ -10099,7 +10117,7 @@
         <v>Oral rehydration salts</v>
       </c>
       <c r="B65" s="98" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="C65" s="25"/>
     </row>
@@ -10109,7 +10127,7 @@
         <v>Public provision of complementary foods</v>
       </c>
       <c r="B66" s="98" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="C66" s="25"/>
     </row>
@@ -10119,7 +10137,7 @@
         <v>Public provision of complementary foods</v>
       </c>
       <c r="B67" s="98" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="C67" s="25"/>
     </row>
@@ -10129,7 +10147,7 @@
         <v>Public provision of complementary foods with iron</v>
       </c>
       <c r="B68" s="98" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="C68" s="25"/>
     </row>
@@ -10139,7 +10157,7 @@
         <v>Public provision of complementary foods with iron</v>
       </c>
       <c r="B69" s="98" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="C69" s="25"/>
     </row>
@@ -10149,7 +10167,7 @@
         <v>Public provision of complementary foods with iron (malaria area)</v>
       </c>
       <c r="B70" s="98" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="C70" s="25"/>
     </row>
@@ -10159,7 +10177,7 @@
         <v>Public provision of complementary foods with iron (malaria area)</v>
       </c>
       <c r="B71" s="98" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="C71" s="25"/>
     </row>
@@ -10169,7 +10187,7 @@
         <v>Sprinkles</v>
       </c>
       <c r="B72" s="98" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="C72" s="25"/>
     </row>
@@ -10179,7 +10197,7 @@
         <v>Sprinkles</v>
       </c>
       <c r="B73" s="98" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="C73" s="25"/>
     </row>
@@ -10189,7 +10207,7 @@
         <v>Sprinkles (malaria area)</v>
       </c>
       <c r="B74" s="98" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="C74" s="25"/>
     </row>
@@ -10199,7 +10217,7 @@
         <v>Sprinkles (malaria area)</v>
       </c>
       <c r="B75" s="98" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="C75" s="25"/>
     </row>
@@ -10209,7 +10227,7 @@
         <v>Treatment of MAM</v>
       </c>
       <c r="B76" s="98" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="C76" s="25"/>
     </row>
@@ -10219,7 +10237,7 @@
         <v>Treatment of MAM</v>
       </c>
       <c r="B77" s="98" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="C77" s="25"/>
     </row>
@@ -10229,7 +10247,7 @@
         <v>Treatment of SAM</v>
       </c>
       <c r="B78" s="98" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="C78" s="25"/>
     </row>
@@ -10239,7 +10257,7 @@
         <v>Treatment of SAM</v>
       </c>
       <c r="B79" s="98" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="C79" s="25"/>
     </row>
@@ -10249,7 +10267,7 @@
         <v>Vitamin A supplementation</v>
       </c>
       <c r="B80" s="98" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="C80" s="25"/>
     </row>
@@ -10259,7 +10277,7 @@
         <v>Vitamin A supplementation</v>
       </c>
       <c r="B81" s="98" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="C81" s="25"/>
     </row>
@@ -10269,7 +10287,7 @@
         <v>WASH: Handwashing</v>
       </c>
       <c r="B82" s="98" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="C82" s="25"/>
     </row>
@@ -10279,7 +10297,7 @@
         <v>WASH: Handwashing</v>
       </c>
       <c r="B83" s="98" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="C83" s="25"/>
     </row>
@@ -10289,7 +10307,7 @@
         <v>WASH: Hygenic disposal</v>
       </c>
       <c r="B84" s="98" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="C84" s="25"/>
     </row>
@@ -10299,7 +10317,7 @@
         <v>WASH: Hygenic disposal</v>
       </c>
       <c r="B85" s="98" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="C85" s="25"/>
     </row>
@@ -10309,7 +10327,7 @@
         <v>WASH: Improved sanitation</v>
       </c>
       <c r="B86" s="98" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="C86" s="25"/>
     </row>
@@ -10319,7 +10337,7 @@
         <v>WASH: Improved sanitation</v>
       </c>
       <c r="B87" s="98" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="C87" s="25"/>
     </row>
@@ -10329,7 +10347,7 @@
         <v>WASH: Improved water source</v>
       </c>
       <c r="B88" s="98" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="C88" s="25"/>
     </row>
@@ -10339,7 +10357,7 @@
         <v>WASH: Improved water source</v>
       </c>
       <c r="B89" s="98" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="C89" s="25"/>
     </row>
@@ -10349,7 +10367,7 @@
         <v>WASH: Piped water</v>
       </c>
       <c r="B90" s="98" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="C90" s="25"/>
     </row>
@@ -10359,7 +10377,7 @@
         <v>WASH: Piped water</v>
       </c>
       <c r="B91" s="98" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="C91" s="25"/>
     </row>
@@ -10369,7 +10387,7 @@
         <v>Zinc for treatment + ORS</v>
       </c>
       <c r="B92" s="98" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="C92" s="25"/>
     </row>
@@ -10379,7 +10397,7 @@
         <v>Zinc for treatment + ORS</v>
       </c>
       <c r="B93" s="98" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="C93" s="25"/>
     </row>
@@ -10389,7 +10407,7 @@
         <v>Zinc supplementation</v>
       </c>
       <c r="B94" s="98" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="C94" s="25"/>
     </row>
@@ -10399,7 +10417,7 @@
         <v>Zinc supplementation</v>
       </c>
       <c r="B95" s="98" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="C95" s="25"/>
     </row>
@@ -10409,7 +10427,7 @@
         <v>IYCF 1</v>
       </c>
       <c r="B96" s="98" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="C96" s="25"/>
     </row>
@@ -10419,7 +10437,7 @@
         <v>IYCF 1</v>
       </c>
       <c r="B97" s="98" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="C97" s="25"/>
     </row>
@@ -10429,7 +10447,7 @@
         <v>IYCF 2</v>
       </c>
       <c r="B98" s="98" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="C98" s="25"/>
     </row>
@@ -10439,7 +10457,7 @@
         <v>IYCF 2</v>
       </c>
       <c r="B99" s="98" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="C99" s="25"/>
     </row>
@@ -10449,7 +10467,7 @@
         <v>IYCF 3</v>
       </c>
       <c r="B100" s="98" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="C100" s="25"/>
     </row>
@@ -10459,7 +10477,7 @@
         <v>IYCF 3</v>
       </c>
       <c r="B101" s="98" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="C101" s="25"/>
     </row>
@@ -10487,7 +10505,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A1" s="7" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="B1" s="7"/>
     </row>
@@ -10508,27 +10526,27 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
     </row>
   </sheetData>
@@ -10544,7 +10562,7 @@
   </sheetPr>
   <dimension ref="A1:E51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -10558,10 +10576,10 @@
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>134</v>
@@ -11305,7 +11323,7 @@
         <v>0.95</v>
       </c>
       <c r="D49" s="124" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
     </row>
     <row r="50" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -11320,7 +11338,7 @@
         <v>0.95</v>
       </c>
       <c r="D50" s="124" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
     </row>
     <row r="51" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -11335,7 +11353,7 @@
         <v>0.95</v>
       </c>
       <c r="D51" s="124" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
     </row>
   </sheetData>
@@ -11367,15 +11385,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A1" s="139" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="B1" s="139" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A2" s="139" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="B2" s="138">
         <v>1000000</v>
@@ -11383,7 +11401,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A3" s="139" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="B3" s="138"/>
     </row>
@@ -11412,10 +11430,10 @@
   <sheetData>
     <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="7" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -13160,6 +13178,11 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="B36:B38"/>
+    <mergeCell ref="B39:B41"/>
+    <mergeCell ref="B42:B44"/>
+    <mergeCell ref="B45:B47"/>
+    <mergeCell ref="B48:B50"/>
     <mergeCell ref="B25:B27"/>
     <mergeCell ref="B28:B30"/>
     <mergeCell ref="B31:B33"/>
@@ -13170,11 +13193,6 @@
     <mergeCell ref="B14:B16"/>
     <mergeCell ref="B19:B21"/>
     <mergeCell ref="B22:B24"/>
-    <mergeCell ref="B36:B38"/>
-    <mergeCell ref="B39:B41"/>
-    <mergeCell ref="B42:B44"/>
-    <mergeCell ref="B45:B47"/>
-    <mergeCell ref="B48:B50"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -13259,7 +13277,7 @@
         <v>13</v>
       </c>
       <c r="B2" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>14</v>
@@ -14187,7 +14205,7 @@
         <v>27</v>
       </c>
       <c r="B24" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="C24" s="4" t="s">
         <v>14</v>
@@ -15113,13 +15131,13 @@
     </row>
     <row r="46" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A46" s="7" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="B46" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="D46" s="112">
         <v>1</v>
@@ -15163,7 +15181,7 @@
     </row>
     <row r="47" spans="1:16" x14ac:dyDescent="0.15">
       <c r="C47" s="4" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="D47" s="112">
         <v>1</v>
@@ -15210,7 +15228,7 @@
         <v>28</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="D48" s="112">
         <v>1</v>
@@ -15254,7 +15272,7 @@
     </row>
     <row r="49" spans="1:16" x14ac:dyDescent="0.15">
       <c r="C49" s="4" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="D49" s="112">
         <v>1</v>
@@ -15301,7 +15319,7 @@
         <v>30</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="D50" s="112">
         <v>1</v>
@@ -15345,7 +15363,7 @@
     </row>
     <row r="51" spans="1:16" x14ac:dyDescent="0.15">
       <c r="C51" s="4" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="D51" s="112">
         <v>1</v>
@@ -15392,7 +15410,7 @@
         <v>31</v>
       </c>
       <c r="C52" s="4" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="D52" s="112">
         <v>1</v>
@@ -15436,7 +15454,7 @@
     </row>
     <row r="53" spans="1:16" x14ac:dyDescent="0.15">
       <c r="C53" s="4" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="D53" s="112">
         <v>1</v>
@@ -15483,7 +15501,7 @@
         <v>35</v>
       </c>
       <c r="C54" s="4" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="D54" s="112">
         <v>1</v>
@@ -15527,7 +15545,7 @@
     </row>
     <row r="55" spans="1:16" x14ac:dyDescent="0.15">
       <c r="C55" s="4" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="D55" s="112">
         <v>1</v>
@@ -15575,7 +15593,7 @@
         <v>79</v>
       </c>
       <c r="C56" s="4" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="D56" s="112">
         <v>1</v>
@@ -15619,7 +15637,7 @@
     </row>
     <row r="57" spans="1:16" x14ac:dyDescent="0.15">
       <c r="C57" s="4" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="D57" s="112">
         <v>1</v>
@@ -15666,7 +15684,7 @@
         <v>80</v>
       </c>
       <c r="C58" s="4" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="D58" s="112">
         <v>1</v>
@@ -15710,7 +15728,7 @@
     </row>
     <row r="59" spans="1:16" x14ac:dyDescent="0.15">
       <c r="C59" s="4" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="D59" s="112">
         <v>1</v>
@@ -15757,7 +15775,7 @@
         <v>81</v>
       </c>
       <c r="C60" s="4" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="D60" s="112">
         <v>1</v>
@@ -15801,7 +15819,7 @@
     </row>
     <row r="61" spans="1:16" x14ac:dyDescent="0.15">
       <c r="C61" s="4" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="D61" s="112">
         <v>1</v>
@@ -15879,7 +15897,7 @@
         <v>36</v>
       </c>
       <c r="B64" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="C64" s="4" t="s">
         <v>37</v>
@@ -16595,7 +16613,7 @@
     </row>
     <row r="80" spans="2:16" x14ac:dyDescent="0.15">
       <c r="B80" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="C80" s="4" t="s">
         <v>37</v>
@@ -17162,10 +17180,10 @@
     </row>
     <row r="94" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A94" s="7" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="B94" s="8" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="C94" s="4" t="s">
         <v>37</v>
@@ -17377,7 +17395,7 @@
         <v>48</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="C1" s="7" t="s">
         <v>6</v>
@@ -17397,7 +17415,7 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A2" s="7" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="B2" t="s">
         <v>59</v>
@@ -17421,10 +17439,10 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A4" s="7" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="C4" s="113">
         <v>1.024</v>
@@ -17555,7 +17573,7 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A12" s="7" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>133</v>
@@ -17661,7 +17679,7 @@
         <v>142</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="C18" s="113">
         <v>1.024</v>
@@ -17684,7 +17702,7 @@
         <v>143</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="C20" s="113">
         <v>1.024</v>
@@ -17704,10 +17722,10 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A22" s="7" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="B22" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="C22" s="33">
         <v>1</v>
@@ -17752,7 +17770,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="B1" s="7" t="s">
         <v>48</v>
@@ -18064,7 +18082,7 @@
         <v>48</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="C1" s="7" t="s">
         <v>6</v>
@@ -18108,7 +18126,7 @@
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A2" s="7" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="B2" s="9" t="s">
         <v>74</v>
@@ -19167,7 +19185,7 @@
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A27" s="7" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="B27" s="4" t="s">
         <v>91</v>
@@ -19385,7 +19403,7 @@
         <v>48</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="C1" s="7" t="s">
         <v>6</v>
@@ -19405,7 +19423,7 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A2" s="7" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="B2" s="33" t="s">
         <v>145</v>
@@ -19428,7 +19446,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A4" s="7" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="B4" s="34" t="s">
         <v>144</v>
@@ -19478,7 +19496,7 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>5</v>
@@ -19507,7 +19525,7 @@
         <v>47</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>96</v>
@@ -19579,7 +19597,7 @@
     <row r="5" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A5" s="8"/>
       <c r="B5" s="33" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="C5" s="34" t="s">
         <v>96</v>
@@ -20115,10 +20133,10 @@
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A28" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="C28" s="4" t="s">
         <v>96</v>
@@ -20182,10 +20200,10 @@
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A31" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="C31" s="4" t="s">
         <v>96</v>
@@ -20249,10 +20267,10 @@
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A34" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="C34" s="4" t="s">
         <v>96</v>
@@ -20316,10 +20334,10 @@
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A37" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="C37" s="4" t="s">
         <v>96</v>
@@ -20383,10 +20401,10 @@
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A40" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="C40" s="4" t="s">
         <v>96</v>
@@ -20453,7 +20471,7 @@
         <v>133</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="C43" s="4" t="s">
         <v>96</v>
@@ -20579,10 +20597,10 @@
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A49" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="C49" s="4" t="s">
         <v>96</v>
@@ -20625,10 +20643,10 @@
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A51" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="C51" s="4" t="s">
         <v>96</v>
@@ -20904,7 +20922,7 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>5</v>
@@ -20928,7 +20946,7 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A2" s="4" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="B2" s="98" t="s">
         <v>82</v>
@@ -20970,7 +20988,7 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A4" s="4" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="B4" t="s">
         <v>82</v>
@@ -21013,7 +21031,7 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A6" s="4" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="B6" t="s">
         <v>82</v>
@@ -21081,25 +21099,25 @@
   <sheetData>
     <row r="1" spans="1:6" ht="65" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="B1" s="89" t="s">
         <v>48</v>
       </c>
       <c r="C1" s="90" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="D1" s="90" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="E1" s="90" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="F1" s="1"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="B2" s="54" t="s">
         <v>51</v>
@@ -21159,10 +21177,10 @@
   <sheetData>
     <row r="1" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A1" s="7" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="C1" s="7">
         <v>2010</v>
@@ -21450,7 +21468,7 @@
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A14" s="7" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="B14" s="7" t="s">
         <v>6</v>
@@ -21629,7 +21647,7 @@
         <v>73</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="C1" s="7" t="s">
         <v>6</v>
@@ -23136,7 +23154,7 @@
     </row>
     <row r="35" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B35" s="33" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="C35" s="3">
         <v>0</v>
@@ -23197,7 +23215,7 @@
         <v>76</v>
       </c>
       <c r="B37" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="C37" s="3">
         <v>1</v>
@@ -23241,7 +23259,7 @@
     </row>
     <row r="38" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B38" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="C38" s="3">
         <v>1</v>
@@ -23285,7 +23303,7 @@
     </row>
     <row r="39" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B39" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="C39" s="3">
         <v>1</v>
@@ -23329,7 +23347,7 @@
     </row>
     <row r="40" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B40" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="C40" s="3">
         <v>1</v>
@@ -23373,7 +23391,7 @@
     </row>
     <row r="41" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B41" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="C41" s="3">
         <v>1</v>
@@ -23417,7 +23435,7 @@
     </row>
     <row r="42" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B42" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="C42" s="3">
         <v>1</v>
@@ -23461,7 +23479,7 @@
     </row>
     <row r="43" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B43" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="C43" s="3">
         <v>1</v>
@@ -23505,7 +23523,7 @@
     </row>
     <row r="44" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B44" s="4" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="C44" s="3">
         <v>0</v>
@@ -23549,7 +23567,7 @@
     </row>
     <row r="45" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B45" s="4" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="C45" s="3">
         <v>0</v>
@@ -23593,7 +23611,7 @@
     </row>
     <row r="46" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B46" s="4" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="C46" s="3">
         <v>0</v>
@@ -23937,7 +23955,7 @@
         <v>73</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="C1" s="7" t="s">
         <v>6</v>
@@ -25518,7 +25536,7 @@
     </row>
     <row r="38" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B38" s="8" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="C38" s="32">
         <v>0</v>
@@ -25581,7 +25599,7 @@
         <v>76</v>
       </c>
       <c r="B40" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="C40" s="32">
         <v>1</v>
@@ -25625,7 +25643,7 @@
     </row>
     <row r="41" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B41" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="C41" s="32">
         <v>1</v>
@@ -25669,7 +25687,7 @@
     </row>
     <row r="42" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B42" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="C42" s="32">
         <v>1</v>
@@ -25713,7 +25731,7 @@
     </row>
     <row r="43" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B43" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="C43" s="32">
         <v>1</v>
@@ -25757,7 +25775,7 @@
     </row>
     <row r="44" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B44" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="C44" s="32">
         <v>1</v>
@@ -25801,7 +25819,7 @@
     </row>
     <row r="45" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B45" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="C45" s="32">
         <v>1</v>
@@ -25845,7 +25863,7 @@
     </row>
     <row r="46" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B46" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="C46" s="32">
         <v>1</v>
@@ -25889,7 +25907,7 @@
     </row>
     <row r="47" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B47" s="4" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="C47" s="32">
         <v>0</v>
@@ -25933,7 +25951,7 @@
     </row>
     <row r="48" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B48" s="4" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="C48" s="32">
         <v>0</v>
@@ -25977,7 +25995,7 @@
     </row>
     <row r="49" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B49" s="4" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="C49" s="32">
         <v>0</v>
@@ -26273,37 +26291,37 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A1" s="7" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="B1" s="7" t="s">
         <v>13</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="F1" s="7" t="s">
         <v>36</v>
       </c>
       <c r="G1" s="7" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="H1" s="7" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="I1" s="7" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="J1" s="7" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="K1" s="7" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.15">
@@ -26867,37 +26885,37 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A1" s="7" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="B1" s="7" t="s">
         <v>13</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="F1" s="7" t="s">
         <v>36</v>
       </c>
       <c r="G1" s="7" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="H1" s="7" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="I1" s="7" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="J1" s="7" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="K1" s="7" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.15">
@@ -27192,7 +27210,7 @@
     </row>
     <row r="2" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="7" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="B2" s="60">
         <v>7.0000000000000001E-3</v>
@@ -27448,7 +27466,7 @@
     </row>
     <row r="10" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="7" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="B10" s="60">
         <v>0</v>
@@ -27481,7 +27499,7 @@
     </row>
     <row r="11" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="7" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="B11" s="60">
         <v>0</v>
@@ -28101,7 +28119,7 @@
     </row>
     <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="4" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="B2" s="12">
         <v>2.4300000000000002</v>
@@ -28121,7 +28139,7 @@
     </row>
     <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="B3" s="22">
         <v>5.1999999999999998E-2</v>
@@ -28241,7 +28259,7 @@
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A1" s="7" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="B1" s="7" t="s">
         <v>12</v>
@@ -28288,10 +28306,10 @@
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A2" s="7" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="B2" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="C2" s="109">
         <f t="shared" ref="C2:O2" si="0">1-C3</f>
@@ -28348,7 +28366,7 @@
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.15">
       <c r="B3" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="C3" s="109">
         <f>C6</f>
@@ -28422,10 +28440,10 @@
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A5" s="7" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="B5" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="C5" s="26">
         <v>0.1</v>
@@ -28469,10 +28487,10 @@
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A6" s="7" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="B6" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="C6" s="26">
         <v>0.05</v>
@@ -28516,10 +28534,10 @@
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A7" s="110" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="B7" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="C7" s="64">
         <v>0.01</v>
@@ -28984,21 +29002,21 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A1" s="7" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="39" x14ac:dyDescent="0.15">
       <c r="A2" s="73" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="B2" s="79" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="C2" s="75">
         <v>0.15</v>
@@ -29006,7 +29024,7 @@
     </row>
     <row r="3" spans="1:3" ht="52" x14ac:dyDescent="0.15">
       <c r="B3" s="74" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="C3" s="75">
         <v>0.03</v>
@@ -29014,7 +29032,7 @@
     </row>
     <row r="4" spans="1:3" ht="52" x14ac:dyDescent="0.15">
       <c r="B4" s="74" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="C4" s="75">
         <v>0</v>
@@ -29022,7 +29040,7 @@
     </row>
     <row r="5" spans="1:3" ht="39" x14ac:dyDescent="0.15">
       <c r="B5" s="76" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="C5" s="75">
         <v>0.19</v>
@@ -29030,7 +29048,7 @@
     </row>
     <row r="6" spans="1:3" ht="52" x14ac:dyDescent="0.15">
       <c r="B6" s="76" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="C6" s="75">
         <v>0.39</v>
@@ -29038,7 +29056,7 @@
     </row>
     <row r="7" spans="1:3" ht="52" x14ac:dyDescent="0.15">
       <c r="B7" s="76" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="C7" s="75">
         <v>0.19</v>
@@ -29046,7 +29064,7 @@
     </row>
     <row r="8" spans="1:3" ht="26" x14ac:dyDescent="0.15">
       <c r="B8" s="77" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="C8" s="75">
         <v>1E-3</v>
@@ -29054,7 +29072,7 @@
     </row>
     <row r="9" spans="1:3" ht="52" x14ac:dyDescent="0.15">
       <c r="B9" s="77" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="C9" s="75">
         <v>7.0000000000000001E-3</v>
@@ -29062,7 +29080,7 @@
     </row>
     <row r="10" spans="1:3" ht="52" x14ac:dyDescent="0.15">
       <c r="B10" s="77" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="C10" s="75">
         <v>0.04</v>
@@ -29073,10 +29091,10 @@
     </row>
     <row r="12" spans="1:3" ht="26" x14ac:dyDescent="0.15">
       <c r="A12" s="73" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="B12" s="78" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="C12" s="75">
         <v>0.34</v>
@@ -29084,7 +29102,7 @@
     </row>
     <row r="13" spans="1:3" ht="26" x14ac:dyDescent="0.15">
       <c r="B13" s="78" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="C13" s="75">
         <v>0.05</v>
@@ -29092,7 +29110,7 @@
     </row>
     <row r="14" spans="1:3" ht="26" x14ac:dyDescent="0.15">
       <c r="B14" s="78" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="C14" s="75">
         <v>7.0000000000000007E-2</v>
@@ -29100,7 +29118,7 @@
     </row>
     <row r="15" spans="1:3" ht="26" x14ac:dyDescent="0.15">
       <c r="B15" s="78" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="C15" s="75">
         <v>0.55000000000000004</v>
@@ -29190,10 +29208,10 @@
     </row>
     <row r="5" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="7" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="B5" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="C5" s="25"/>
       <c r="D5" s="113">
@@ -29208,7 +29226,7 @@
     </row>
     <row r="6" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="C6" s="120">
         <v>1</v>
@@ -29270,10 +29288,10 @@
     </row>
     <row r="11" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="7" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="C11" s="126">
         <v>1</v>
@@ -29412,10 +29430,10 @@
     </row>
     <row r="21" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="7" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="B21" s="80" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="C21" s="127">
         <v>1</v>
@@ -29433,7 +29451,7 @@
     </row>
     <row r="22" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B22" s="80" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="C22" s="127">
         <v>1</v>
@@ -29451,7 +29469,7 @@
     </row>
     <row r="23" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B23" s="80" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="C23" s="127">
         <v>1</v>
@@ -29469,7 +29487,7 @@
     </row>
     <row r="24" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B24" s="83" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="C24" s="127">
         <v>1</v>
@@ -29487,7 +29505,7 @@
     </row>
     <row r="25" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B25" s="83" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="C25" s="127">
         <v>1</v>
@@ -29505,7 +29523,7 @@
     </row>
     <row r="26" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B26" s="83" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="C26" s="127">
         <v>1</v>
@@ -29523,7 +29541,7 @@
     </row>
     <row r="27" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B27" s="84" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="C27" s="127">
         <v>1</v>
@@ -29541,7 +29559,7 @@
     </row>
     <row r="28" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B28" s="84" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="C28" s="127">
         <v>1</v>
@@ -29559,7 +29577,7 @@
     </row>
     <row r="29" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B29" s="84" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="C29" s="127">
         <v>1</v>
@@ -29593,10 +29611,10 @@
     </row>
     <row r="32" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A32" s="7" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="B32" s="86" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="C32" s="127">
         <v>1</v>
@@ -29614,7 +29632,7 @@
     </row>
     <row r="33" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B33" s="86" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="C33" s="127">
         <v>1</v>
@@ -29632,7 +29650,7 @@
     </row>
     <row r="34" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B34" s="86" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="C34" s="127">
         <v>1</v>
@@ -29650,7 +29668,7 @@
     </row>
     <row r="35" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B35" s="86" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="C35" s="127">
         <v>1</v>

</xml_diff>

<commit_message>
Updated impacted pop to include 1-6 months
</commit_message>
<xml_diff>
--- a/input_spreadsheets/Master/InputForCode_Master.xlsx
+++ b/input_spreadsheets/Master/InputForCode_Master.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/samhainsworth/Desktop/Github Projects/Nutrition/input_spreadsheets/Master/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{15ED079D-C42F-4E42-ACDE-8DFDD31FD4CC}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{5E9BB785-C909-1F45-8469-A7C56A6C9C87}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" tabRatio="500" firstSheet="6" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" tabRatio="500" firstSheet="25" activeTab="30" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Baseline year demographics" sheetId="1" r:id="rId1"/>
@@ -8188,7 +8188,7 @@
   </sheetPr>
   <dimension ref="A1:B52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
@@ -8542,7 +8542,7 @@
   <dimension ref="A1:C52"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -8938,7 +8938,7 @@
   <dimension ref="A1:B52"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A29" sqref="A29"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -9427,8 +9427,8 @@
   </sheetPr>
   <dimension ref="A1:Y103"/>
   <sheetViews>
-    <sheetView topLeftCell="A35" workbookViewId="0">
-      <selection activeCell="A57" sqref="A57"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -10612,7 +10612,7 @@
   <dimension ref="A1:E52"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A29" sqref="A29"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -18126,8 +18126,8 @@
   </sheetPr>
   <dimension ref="A1:O41"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C26" sqref="C26:D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -19255,7 +19255,7 @@
       <c r="C26" s="33">
         <v>1</v>
       </c>
-      <c r="D26" s="113">
+      <c r="D26" s="33">
         <v>1</v>
       </c>
       <c r="E26" s="113">
@@ -21735,8 +21735,8 @@
   </sheetPr>
   <dimension ref="A1:O52"/>
   <sheetViews>
-    <sheetView topLeftCell="A27" zoomScale="85" zoomScaleNormal="118" workbookViewId="0">
-      <selection activeCell="B48" sqref="B48"/>
+    <sheetView zoomScale="85" zoomScaleNormal="118" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -24087,8 +24087,8 @@
   </sheetPr>
   <dimension ref="A1:O55"/>
   <sheetViews>
-    <sheetView topLeftCell="A33" workbookViewId="0">
-      <selection activeCell="B51" sqref="B51"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -24601,7 +24601,7 @@
         <v>1</v>
       </c>
       <c r="D12" s="92">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E12" s="92">
         <v>0</v>

</xml_diff>